<commit_message>
Kapitel Material wurde fertiggestellt
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/samuel_egli_ksbg_ch/Documents/1/4. Kanti/Maturaarbeit/Arbeit/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1200FC4-8803-46EB-A19D-575AFBCC1C09}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A64FF50C-4A65-4BC0-A464-389E9324E554}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fehlerrechnung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tröpfchen</t>
   </si>
@@ -88,6 +89,51 @@
   <si>
     <t>rel</t>
   </si>
+  <si>
+    <t>Elektrisches Feld [V/m]</t>
+  </si>
+  <si>
+    <t>Steigezeit [s]</t>
+  </si>
+  <si>
+    <t>Sinkzeit [s]</t>
+  </si>
+  <si>
+    <t>Distanz [m]</t>
+  </si>
+  <si>
+    <t>Steiggeschwindigkeit [m/s]</t>
+  </si>
+  <si>
+    <t>Sinkgeschwindigkeit [m/s]</t>
+  </si>
+  <si>
+    <t>Luftdruck [Pa]</t>
+  </si>
+  <si>
+    <t>Zähigkeit [Ns/m^2]</t>
+  </si>
+  <si>
+    <t>Dichte [kg/m^3]</t>
+  </si>
+  <si>
+    <t>Fallbeschleunigung</t>
+  </si>
+  <si>
+    <t>Konstante b</t>
+  </si>
+  <si>
+    <t>Messwert</t>
+  </si>
+  <si>
+    <t>absoluter Fehler</t>
+  </si>
+  <si>
+    <t>relativer Fehler [%]</t>
+  </si>
+  <si>
+    <t>elektrischesFeld</t>
+  </si>
 </sst>
 </file>
 
@@ -110,7 +156,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,18 +165,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -156,52 +196,29 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1461,16 +1478,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>158971</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>55226</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>503842</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>221359</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>20487</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1182415</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>98533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1821,19 +1838,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K39" zoomScale="161" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView topLeftCell="C1" zoomScale="65" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="11" width="20.73046875" customWidth="1"/>
-    <col min="12" max="12" width="20.73046875" style="8" customWidth="1"/>
+    <col min="1" max="10" width="20.73046875" customWidth="1"/>
+    <col min="11" max="11" width="20.73046875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="20.73046875" style="10" customWidth="1"/>
     <col min="13" max="14" width="20.73046875" customWidth="1"/>
     <col min="16" max="16" width="11.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1867,15 +1885,17 @@
       <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
+      <c r="N1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
       <c r="Q1"/>
       <c r="R1"/>
       <c r="S1"/>
@@ -1889,331 +1909,376 @@
       <c r="AA1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>2.11954217888936E-5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="8">
         <v>2.0080321285139999E-4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>23.59</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="6">
         <v>585</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H2" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J2">
-        <v>886</v>
-      </c>
-      <c r="K2">
+      <c r="H2" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I2" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J2" s="6">
+        <v>886</v>
+      </c>
+      <c r="K2" s="6">
         <v>94364</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="10">
         <v>3.2747980958213941E-19</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="6">
         <v>2</v>
       </c>
+      <c r="N2" s="8">
+        <f>F2/H2</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>2.158894645941278E-5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="8">
         <v>8.4602368866328257E-5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>23.16</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>5.91</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>585</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H3" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J3">
-        <v>886</v>
-      </c>
-      <c r="K3">
+      <c r="H3" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I3" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J3" s="6">
+        <v>886</v>
+      </c>
+      <c r="K3" s="6">
         <v>94364</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="10">
         <v>1.5851685892692281E-19</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="6">
         <v>1</v>
       </c>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N48" si="0">F3/H3</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>1.9833399444664819E-5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>8.6805555555555559E-5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>25.21</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>5.76</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>585</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H4" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I4" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J4">
-        <v>886</v>
-      </c>
-      <c r="K4">
+      <c r="H4" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J4" s="6">
+        <v>886</v>
+      </c>
+      <c r="K4" s="6">
         <v>94364</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="10">
         <v>1.5068138364557E-19</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="6">
         <v>1</v>
       </c>
+      <c r="N4" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>2.4715768660405332E-5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>9.3808630393996234E-5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>20.23</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>5.33</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>585</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H5" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I5" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J5">
-        <v>886</v>
-      </c>
-      <c r="K5">
+      <c r="H5" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J5" s="6">
+        <v>886</v>
+      </c>
+      <c r="K5" s="6">
         <v>94364</v>
       </c>
-      <c r="L5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>2.04164965291956E-5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="8">
         <f>0.0005/E6</f>
         <v>8.9126559714795006E-5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>24.49</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>5.61</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>585</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H6" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I6" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J6">
-        <v>886</v>
-      </c>
-      <c r="K6">
+      <c r="H6" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I6" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>886</v>
+      </c>
+      <c r="K6" s="6">
         <v>94364</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="10">
         <v>1.5772476256952349E-19</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="6">
         <v>1</v>
       </c>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>1.975503753457132E-5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>1.9685039370070001E-4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>25.31</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>2.54</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>585</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H7" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I7" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J7">
-        <v>886</v>
-      </c>
-      <c r="K7">
+      <c r="H7" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I7" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J7" s="6">
+        <v>886</v>
+      </c>
+      <c r="K7" s="6">
         <v>94364</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="10">
         <v>3.052773302419662E-19</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="6">
         <v>2</v>
       </c>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="8">
         <v>2.044153720359771E-5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="8">
         <v>1.97628458498E-4</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>24.46</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>2.5299999999999998</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>585</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H8" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J8">
-        <v>886</v>
-      </c>
-      <c r="K8">
+      <c r="H8" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I8" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>886</v>
+      </c>
+      <c r="K8" s="6">
         <v>94364</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="10">
         <v>3.1423605559845701E-19</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="8">
         <v>1.8429782528566169E-5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
         <v>9.328358208955224E-5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>27.13</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>5.36</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>585</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="9">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H9" s="4">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I9" s="4">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J9" s="3">
-        <v>886</v>
-      </c>
-      <c r="K9">
+      <c r="H9" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I9" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J9" s="6">
+        <v>886</v>
+      </c>
+      <c r="K9" s="6">
         <v>94364</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="10">
         <v>1.5046225734477661E-19</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="6">
         <v>1</v>
       </c>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
@@ -2227,284 +2292,323 @@
       <c r="AA9"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="8">
         <v>1.708817498291182E-5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="8">
         <v>1.2562814070350001E-4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>29.26</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>3.98</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>586</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H10" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I10" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J10">
-        <v>886</v>
-      </c>
-      <c r="K10">
+      <c r="H10" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I10" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J10" s="6">
+        <v>886</v>
+      </c>
+      <c r="K10" s="6">
         <v>94364</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="10">
         <v>1.8492070982804951E-19</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="6">
         <v>1</v>
       </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="8">
         <v>1.692620176032498E-5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="8">
         <v>3.9062500000000002E-4</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>29.54</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>1.28</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>586</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H11" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I11" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J11">
-        <v>886</v>
-      </c>
-      <c r="K11">
+      <c r="H11" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I11" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>886</v>
+      </c>
+      <c r="K11" s="6">
         <v>94364</v>
       </c>
-      <c r="L11"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="8">
         <v>1.2333497779970399E-5</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="8">
         <v>1.121076233183E-4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>40.54</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>4.46</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>586</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H12" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I12" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J12">
-        <v>886</v>
-      </c>
-      <c r="K12">
+      <c r="H12" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I12" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J12" s="6">
+        <v>886</v>
+      </c>
+      <c r="K12" s="6">
         <v>94364</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="10">
         <v>1.2938659935743371E-19</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="6">
         <v>1</v>
       </c>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>1.289324394017535E-5</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="8">
         <v>1.295336787564E-4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>38.78</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>3.86</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>586</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H13" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I13" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J13">
-        <v>886</v>
-      </c>
-      <c r="K13">
+      <c r="H13" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I13" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J13" s="6">
+        <v>886</v>
+      </c>
+      <c r="K13" s="6">
         <v>94364</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="10">
         <v>1.5267483032452281E-19</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="6">
         <v>1</v>
       </c>
+      <c r="N13" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="8">
         <v>1.316135825217162E-5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="8">
         <v>2.2624434389139999E-4</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>37.99</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>2.21</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>586</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H14" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I14" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J14">
-        <v>886</v>
-      </c>
-      <c r="K14">
+      <c r="H14" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I14" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J14" s="6">
+        <v>886</v>
+      </c>
+      <c r="K14" s="6">
         <v>94364</v>
       </c>
-      <c r="L14"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="8">
         <v>1.151012891344383E-5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="8">
         <v>1.262626262626E-4</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>43.44</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>3.96</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <v>586</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H15" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I15" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J15">
-        <v>886</v>
-      </c>
-      <c r="K15">
+      <c r="H15" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I15" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J15" s="6">
+        <v>886</v>
+      </c>
+      <c r="K15" s="6">
         <v>94364</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="10">
         <v>1.365537769282638E-19</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+      <c r="N15" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="8">
         <v>1.575299306868305E-5</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="8">
         <v>1.210653753026E-4</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>31.74</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>4.13</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="6">
         <v>586</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="9">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H16" s="4">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I16" s="4">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J16" s="3">
-        <v>886</v>
-      </c>
-      <c r="K16">
+      <c r="H16" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I16" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J16" s="6">
+        <v>886</v>
+      </c>
+      <c r="K16" s="6">
         <v>94364</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="10">
         <v>1.679480167697637E-19</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="6">
         <v>1</v>
       </c>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
+      <c r="N16" s="8">
+        <f t="shared" si="0"/>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
       <c r="Q16"/>
       <c r="R16"/>
       <c r="S16"/>
@@ -2518,203 +2622,230 @@
       <c r="AA16"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A17">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="8">
         <v>1.8109380659181451E-5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="8">
         <v>2.2624434389139999E-4</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>27.61</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>2.21</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <v>580</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="9">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H17" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I17" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J17">
-        <v>886</v>
-      </c>
-      <c r="K17">
+      <c r="H17" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I17" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J17" s="6">
+        <v>886</v>
+      </c>
+      <c r="K17" s="6">
         <v>94364</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="10">
         <v>3.3115626946853271E-19</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="6">
         <v>2</v>
       </c>
+      <c r="N17" s="8">
+        <f t="shared" si="0"/>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A18">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="8">
         <v>1.212709192335678E-5</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="8">
         <v>4.5045045045039999E-4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>41.23</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <v>580</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="9">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H18" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I18" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J18">
-        <v>886</v>
-      </c>
-      <c r="K18">
+      <c r="H18" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I18" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J18" s="6">
+        <v>886</v>
+      </c>
+      <c r="K18" s="6">
         <v>94364</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="10">
         <v>4.7852879920201003E-19</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="6">
         <v>3</v>
       </c>
+      <c r="N18" s="8">
+        <f t="shared" si="0"/>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A19">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="8">
         <v>1.07781849536538E-5</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="8">
         <v>4.5045045045039999E-4</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>46.39</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <v>580</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="9">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H19" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I19" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J19">
-        <v>886</v>
-      </c>
-      <c r="K19">
+      <c r="H19" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I19" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J19" s="6">
+        <v>886</v>
+      </c>
+      <c r="K19" s="6">
         <v>94364</v>
       </c>
-      <c r="L19"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="8">
+        <f t="shared" si="0"/>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A20">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="8">
         <v>1.065189603749468E-5</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="8">
         <v>2.8409090909090002E-4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>46.94</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <v>1.76</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <v>580</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="9">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H20" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I20" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J20">
-        <v>886</v>
-      </c>
-      <c r="K20">
+      <c r="H20" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I20" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J20" s="6">
+        <v>886</v>
+      </c>
+      <c r="K20" s="6">
         <v>94364</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="10">
         <v>2.7853483615976351E-19</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
+      <c r="N20" s="8">
+        <f t="shared" si="0"/>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="8">
         <v>1.147842056932966E-5</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="8">
         <v>5.6179775280890002E-4</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="6">
         <v>43.56</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="6">
         <v>0.89</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="6">
         <v>580</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="9">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H21" s="4">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I21" s="4">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J21" s="3">
-        <v>886</v>
-      </c>
-      <c r="K21">
+      <c r="H21" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I21" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J21" s="6">
+        <v>886</v>
+      </c>
+      <c r="K21" s="6">
         <v>94364</v>
       </c>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="8">
+        <f t="shared" si="0"/>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
       <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
@@ -2728,249 +2859,285 @@
       <c r="AA21"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A22">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="8">
         <v>1.11656989727557E-5</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="8">
         <v>1.179245283018E-4</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>44.78</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <v>4.24</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <v>583</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H22" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I22" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J22">
-        <v>886</v>
-      </c>
-      <c r="K22">
+      <c r="H22" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I22" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J22" s="6">
+        <v>886</v>
+      </c>
+      <c r="K22" s="6">
         <v>94364</v>
       </c>
-      <c r="L22"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A23">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="8">
         <v>1.4033118158854901E-5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="8">
         <v>2.427184466019E-4</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>35.630000000000003</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <v>2.06</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <v>583</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H23" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J23">
-        <v>886</v>
-      </c>
-      <c r="K23">
+      <c r="H23" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I23" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J23" s="6">
+        <v>886</v>
+      </c>
+      <c r="K23" s="6">
         <v>94364</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="10">
         <v>2.9254518781664188E-19</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="6">
         <v>2</v>
       </c>
+      <c r="N23" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A24">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="8">
         <v>1.282380097460887E-5</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="8">
         <v>1.2562814070350001E-4</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>38.99</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="6">
         <v>3.98</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <v>583</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H24" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I24" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J24">
-        <v>886</v>
-      </c>
-      <c r="K24">
+      <c r="H24" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I24" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J24" s="6">
+        <v>886</v>
+      </c>
+      <c r="K24" s="6">
         <v>94364</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="10">
         <v>1.483515883555309E-19</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="6">
         <v>1</v>
       </c>
+      <c r="N24" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A25">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="8">
         <v>1.304461257500652E-5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="8">
         <v>3.9682539682530001E-4</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>38.33</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="6">
         <v>1.26</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <v>583</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H25" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I25" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J25">
-        <v>886</v>
-      </c>
-      <c r="K25">
+      <c r="H25" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I25" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J25" s="6">
+        <v>886</v>
+      </c>
+      <c r="K25" s="6">
         <v>94364</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="10">
         <v>4.4434402544902837E-19</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="6">
         <v>3</v>
       </c>
+      <c r="N25" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A26">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="8">
         <v>1.446759259259259E-5</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="8">
         <v>2.4875621890539998E-4</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>34.56</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="6">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <v>583</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H26" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I26" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J26">
-        <v>886</v>
-      </c>
-      <c r="K26">
+      <c r="H26" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I26" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J26" s="6">
+        <v>886</v>
+      </c>
+      <c r="K26" s="6">
         <v>94364</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="10">
         <v>3.0617078747401381E-19</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="6">
         <v>2</v>
       </c>
+      <c r="N26" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A27">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="8">
         <v>1.032204789430223E-5</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="8">
         <v>2.3923444976069999E-4</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>48.44</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="6">
         <v>2.09</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <v>583</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H27" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I27" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J27">
-        <v>886</v>
-      </c>
-      <c r="K27">
+      <c r="H27" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I27" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J27" s="6">
+        <v>886</v>
+      </c>
+      <c r="K27" s="6">
         <v>94364</v>
       </c>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:27" s="6" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M27" s="6"/>
+      <c r="N27" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+    </row>
+    <row r="28" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>1.047339757017176E-5</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="8">
         <v>2.6178010471200001E-4</v>
       </c>
       <c r="D28" s="6">
@@ -2982,13 +3149,13 @@
       <c r="F28" s="6">
         <v>583</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H28" s="10">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I28" s="10">
+      <c r="H28" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I28" s="8">
         <v>8.2000000000000007E-3</v>
       </c>
       <c r="J28" s="6">
@@ -2997,904 +3164,1052 @@
       <c r="K28" s="6">
         <v>94364</v>
       </c>
+      <c r="L28" s="10"/>
+      <c r="N28" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A29">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="8">
         <f>0.0005/D29</f>
         <v>3.6284470246734402E-5</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="8">
         <f>0.0005/E29</f>
         <v>3.048780487804878E-4</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>13.78</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <v>1.64</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="6">
         <v>583</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H29" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I29" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J29">
-        <v>886</v>
-      </c>
-      <c r="K29">
+      <c r="H29" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I29" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J29" s="6">
+        <v>886</v>
+      </c>
+      <c r="K29" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L29"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A30">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
-        <f t="shared" ref="B30:B40" si="0">0.0005/D30</f>
+      <c r="B30" s="8">
+        <f t="shared" ref="B30:B40" si="1">0.0005/D30</f>
         <v>3.3579583613163193E-5</v>
       </c>
-      <c r="C30" s="1">
-        <f t="shared" ref="C30:C40" si="1">0.0005/E30</f>
+      <c r="C30" s="8">
+        <f t="shared" ref="C30:C40" si="2">0.0005/E30</f>
         <v>3.95882818685669E-5</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>14.89</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <v>12.63</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="6">
         <v>583</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H30" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I30" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J30">
-        <v>886</v>
-      </c>
-      <c r="K30">
+      <c r="H30" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I30" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J30" s="6">
+        <v>886</v>
+      </c>
+      <c r="K30" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="10">
         <v>1.4554623175668291E-19</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="6">
         <v>1</v>
       </c>
+      <c r="N30" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A31">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <f t="shared" si="0"/>
+      <c r="B31" s="8">
+        <f t="shared" si="1"/>
         <v>1.4744913005013272E-5</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0438413361169103E-4</v>
+      </c>
+      <c r="D31" s="6">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="E31" s="6">
+        <v>4.79</v>
+      </c>
+      <c r="F31" s="6">
+        <v>583</v>
+      </c>
+      <c r="G31" s="9">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H31" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I31" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J31" s="6">
+        <v>886</v>
+      </c>
+      <c r="K31" s="6">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="L31" s="10">
+        <v>1.3963446372113281E-19</v>
+      </c>
+      <c r="M31" s="6">
+        <v>1</v>
+      </c>
+      <c r="N31" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8">
         <f t="shared" si="1"/>
-        <v>1.0438413361169103E-4</v>
-      </c>
-      <c r="D31">
-        <v>33.909999999999997</v>
-      </c>
-      <c r="E31">
-        <v>4.79</v>
-      </c>
-      <c r="F31">
+        <v>2.8851702250432778E-5</v>
+      </c>
+      <c r="C32" s="8">
+        <f t="shared" si="2"/>
+        <v>5.2192066805845514E-5</v>
+      </c>
+      <c r="D32" s="6">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="E32" s="6">
+        <v>9.58</v>
+      </c>
+      <c r="F32" s="6">
         <v>583</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G32" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H31" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I31" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J31">
-        <v>886</v>
-      </c>
-      <c r="K31">
+      <c r="H32" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I32" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J32" s="6">
+        <v>886</v>
+      </c>
+      <c r="K32" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L31">
-        <v>1.3963446372113281E-19</v>
-      </c>
-      <c r="M31">
+      <c r="L32" s="10">
+        <v>1.4673753039611549E-19</v>
+      </c>
+      <c r="M32" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8851702250432778E-5</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="N32" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8">
         <f t="shared" si="1"/>
-        <v>5.2192066805845514E-5</v>
-      </c>
-      <c r="D32">
-        <v>17.329999999999998</v>
-      </c>
-      <c r="E32">
-        <v>9.58</v>
-      </c>
-      <c r="F32">
+        <v>3.0618493570116355E-5</v>
+      </c>
+      <c r="C33" s="8">
+        <f t="shared" si="2"/>
+        <v>5.3995680345572353E-5</v>
+      </c>
+      <c r="D33" s="6">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="E33" s="6">
+        <v>9.26</v>
+      </c>
+      <c r="F33" s="6">
         <v>583</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G33" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H32" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I32" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J32">
-        <v>886</v>
-      </c>
-      <c r="K32">
+      <c r="H33" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I33" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J33" s="6">
+        <v>886</v>
+      </c>
+      <c r="K33" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L32">
-        <v>1.4673753039611549E-19</v>
-      </c>
-      <c r="M32">
+      <c r="L33" s="10">
+        <v>1.5897872941404839E-19</v>
+      </c>
+      <c r="M33" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0618493570116355E-5</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="N33" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8">
         <f t="shared" si="1"/>
-        <v>5.3995680345572353E-5</v>
-      </c>
-      <c r="D33">
-        <v>16.329999999999998</v>
-      </c>
-      <c r="E33">
-        <v>9.26</v>
-      </c>
-      <c r="F33">
+        <v>2.6695141484249868E-5</v>
+      </c>
+      <c r="C34" s="8">
+        <f t="shared" si="2"/>
+        <v>5.8207217694994179E-5</v>
+      </c>
+      <c r="D34" s="6">
+        <v>18.73</v>
+      </c>
+      <c r="E34" s="6">
+        <v>8.59</v>
+      </c>
+      <c r="F34" s="6">
         <v>583</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G34" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H33" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I33" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J33">
-        <v>886</v>
-      </c>
-      <c r="K33">
+      <c r="H34" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I34" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J34" s="6">
+        <v>886</v>
+      </c>
+      <c r="K34" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L33">
-        <v>1.5897872941404839E-19</v>
-      </c>
-      <c r="M33">
+      <c r="L34" s="10">
+        <v>1.4641553540058561E-19</v>
+      </c>
+      <c r="M34" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
-        <f t="shared" si="0"/>
-        <v>2.6695141484249868E-5</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="N34" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8">
         <f t="shared" si="1"/>
-        <v>5.8207217694994179E-5</v>
-      </c>
-      <c r="D34">
-        <v>18.73</v>
-      </c>
-      <c r="E34">
-        <v>8.59</v>
-      </c>
-      <c r="F34">
+        <v>2.9779630732578919E-5</v>
+      </c>
+      <c r="C35" s="8">
+        <f t="shared" si="2"/>
+        <v>5.3418803418803426E-5</v>
+      </c>
+      <c r="D35" s="6">
+        <v>16.79</v>
+      </c>
+      <c r="E35" s="6">
+        <v>9.36</v>
+      </c>
+      <c r="F35" s="6">
         <v>583</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G35" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H34" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I34" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J34">
-        <v>886</v>
-      </c>
-      <c r="K34">
+      <c r="H35" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I35" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J35" s="6">
+        <v>886</v>
+      </c>
+      <c r="K35" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L34">
-        <v>1.4641553540058561E-19</v>
-      </c>
-      <c r="M34">
+      <c r="L35" s="10">
+        <v>1.536419009789623E-19</v>
+      </c>
+      <c r="M35" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <f t="shared" si="0"/>
-        <v>2.9779630732578919E-5</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="N35" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8">
         <f t="shared" si="1"/>
-        <v>5.3418803418803426E-5</v>
-      </c>
-      <c r="D35">
-        <v>16.79</v>
-      </c>
-      <c r="E35">
-        <v>9.36</v>
-      </c>
-      <c r="F35">
+        <v>2.7917364600781685E-5</v>
+      </c>
+      <c r="C36" s="8">
+        <f t="shared" si="2"/>
+        <v>5.76036866359447E-5</v>
+      </c>
+      <c r="D36" s="6">
+        <v>17.91</v>
+      </c>
+      <c r="E36" s="6">
+        <v>8.68</v>
+      </c>
+      <c r="F36" s="6">
         <v>583</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G36" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H35" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I35" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J35">
-        <v>886</v>
-      </c>
-      <c r="K35">
+      <c r="H36" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I36" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J36" s="6">
+        <v>886</v>
+      </c>
+      <c r="K36" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L35">
-        <v>1.536419009789623E-19</v>
-      </c>
-      <c r="M35">
+      <c r="L36" s="10">
+        <v>1.5168780241725071E-19</v>
+      </c>
+      <c r="M36" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <f t="shared" si="0"/>
-        <v>2.7917364600781685E-5</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="N36" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8">
         <f t="shared" si="1"/>
-        <v>5.76036866359447E-5</v>
-      </c>
-      <c r="D36">
-        <v>17.91</v>
-      </c>
-      <c r="E36">
-        <v>8.68</v>
-      </c>
-      <c r="F36">
+        <v>3.0138637733574443E-5</v>
+      </c>
+      <c r="C37" s="8">
+        <f t="shared" si="2"/>
+        <v>5.8072009291521493E-5</v>
+      </c>
+      <c r="D37" s="6">
+        <v>16.59</v>
+      </c>
+      <c r="E37" s="6">
+        <v>8.61</v>
+      </c>
+      <c r="F37" s="6">
         <v>583</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G37" s="9">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H36" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I36" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J36">
-        <v>886</v>
-      </c>
-      <c r="K36">
+      <c r="H37" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I37" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J37" s="6">
+        <v>886</v>
+      </c>
+      <c r="K37" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L36">
-        <v>1.5168780241725071E-19</v>
-      </c>
-      <c r="M36">
+      <c r="L37" s="10">
+        <v>1.641171292859742E-19</v>
+      </c>
+      <c r="M37" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <f t="shared" si="0"/>
-        <v>3.0138637733574443E-5</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="N37" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8">
         <f t="shared" si="1"/>
-        <v>5.8072009291521493E-5</v>
-      </c>
-      <c r="D37">
-        <v>16.59</v>
-      </c>
-      <c r="E37">
-        <v>8.61</v>
-      </c>
-      <c r="F37">
-        <v>583</v>
-      </c>
-      <c r="G37" s="2">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H37" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I37" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J37">
-        <v>886</v>
-      </c>
-      <c r="K37">
+        <v>1.8946570670708603E-5</v>
+      </c>
+      <c r="C38" s="8">
+        <f t="shared" si="2"/>
+        <v>5.3191489361702129E-4</v>
+      </c>
+      <c r="D38" s="6">
+        <v>26.39</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.94</v>
+      </c>
+      <c r="F38" s="6">
+        <v>582</v>
+      </c>
+      <c r="G38" s="8">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H38" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I38" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J38" s="6">
+        <v>886</v>
+      </c>
+      <c r="K38" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L37">
-        <v>1.641171292859742E-19</v>
-      </c>
-      <c r="M37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1">
-        <f t="shared" si="0"/>
-        <v>1.8946570670708603E-5</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="L38" s="10">
+        <v>7.6660747025858679E-19</v>
+      </c>
+      <c r="M38" s="6">
+        <v>5</v>
+      </c>
+      <c r="N38" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8">
         <f t="shared" si="1"/>
-        <v>5.3191489361702129E-4</v>
-      </c>
-      <c r="D38">
-        <v>26.39</v>
-      </c>
-      <c r="E38">
-        <v>0.94</v>
-      </c>
-      <c r="F38">
+        <v>1.8982536066818528E-5</v>
+      </c>
+      <c r="C39" s="8">
+        <f t="shared" si="2"/>
+        <v>3.5460992907801421E-4</v>
+      </c>
+      <c r="D39" s="6">
+        <v>26.34</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="F39" s="6">
         <v>582</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G39" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H38" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I38" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J38">
-        <v>886</v>
-      </c>
-      <c r="K38">
+      <c r="H39" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I39" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J39" s="6">
+        <v>886</v>
+      </c>
+      <c r="K39" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L38">
-        <v>7.6660747025858679E-19</v>
-      </c>
-      <c r="M38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1">
-        <f t="shared" si="0"/>
-        <v>1.8982536066818528E-5</v>
-      </c>
-      <c r="C39" s="1">
+      <c r="L39" s="10">
+        <v>5.2055514577343985E-19</v>
+      </c>
+      <c r="M39" s="6">
+        <v>3</v>
+      </c>
+      <c r="N39" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8">
         <f t="shared" si="1"/>
-        <v>3.5460992907801421E-4</v>
-      </c>
-      <c r="D39">
-        <v>26.34</v>
-      </c>
-      <c r="E39">
-        <v>1.41</v>
-      </c>
-      <c r="F39">
+        <v>1.6539861065167053E-5</v>
+      </c>
+      <c r="C40" s="8">
+        <f t="shared" si="2"/>
+        <v>3.3112582781456954E-4</v>
+      </c>
+      <c r="D40" s="6">
+        <v>30.23</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="F40" s="6">
         <v>582</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G40" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H39" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I39" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J39">
-        <v>886</v>
-      </c>
-      <c r="K39">
+      <c r="H40" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I40" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J40" s="6">
+        <v>886</v>
+      </c>
+      <c r="K40" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L39">
-        <v>5.2055514577343985E-19</v>
-      </c>
-      <c r="M39">
+      <c r="L40" s="10">
+        <v>4.4242549593716838E-19</v>
+      </c>
+      <c r="M40" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6539861065167053E-5</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="1"/>
-        <v>3.3112582781456954E-4</v>
-      </c>
-      <c r="D40">
-        <v>30.23</v>
-      </c>
-      <c r="E40">
-        <v>1.51</v>
-      </c>
-      <c r="F40">
-        <v>582</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H40" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I40" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J40">
-        <v>886</v>
-      </c>
-      <c r="K40">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L40">
-        <v>4.4242549593716838E-19</v>
-      </c>
-      <c r="M40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A41">
+      <c r="N40" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="8">
         <f>0.0005/D41</f>
         <v>1.7768301350390903E-5</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="8">
         <f>0.0005/E41</f>
         <v>4.8543689320388347E-4</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>28.14</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="6">
         <v>1.03</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="6">
         <v>582</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H41" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I41" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J41">
-        <v>886</v>
-      </c>
-      <c r="K41">
+      <c r="H41" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I41" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J41" s="6">
+        <v>886</v>
+      </c>
+      <c r="K41" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="10">
         <v>6.7141516307161576E-19</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A42">
+      <c r="N41" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
-        <f t="shared" ref="B42:B48" si="2">0.0005/D42</f>
+      <c r="B42" s="8">
+        <f t="shared" ref="B42:B48" si="3">0.0005/D42</f>
         <v>1.4667057788207684E-5</v>
       </c>
-      <c r="C42" s="1">
-        <f t="shared" ref="C42:C48" si="3">0.0005/E42</f>
+      <c r="C42" s="8">
+        <f t="shared" ref="C42:C48" si="4">0.0005/E42</f>
         <v>3.4965034965034965E-4</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>34.090000000000003</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="6">
         <v>1.43</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="6">
         <v>582</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H42" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I42" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J42">
-        <v>886</v>
-      </c>
-      <c r="K42">
+      <c r="H42" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I42" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J42" s="6">
+        <v>886</v>
+      </c>
+      <c r="K42" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L42"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A43">
+      <c r="M42" s="6"/>
+      <c r="N42" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
-        <f t="shared" si="2"/>
+      <c r="B43" s="8">
+        <f t="shared" si="3"/>
         <v>1.4912019087384431E-5</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="8">
+        <f t="shared" si="4"/>
+        <v>2.0746887966804979E-4</v>
+      </c>
+      <c r="D43" s="6">
+        <v>33.53</v>
+      </c>
+      <c r="E43" s="6">
+        <v>2.41</v>
+      </c>
+      <c r="F43" s="6">
+        <v>582</v>
+      </c>
+      <c r="G43" s="8">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H43" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I43" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J43" s="6">
+        <v>886</v>
+      </c>
+      <c r="K43" s="6">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M43" s="6"/>
+      <c r="N43" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8">
         <f t="shared" si="3"/>
-        <v>2.0746887966804979E-4</v>
-      </c>
-      <c r="D43">
-        <v>33.53</v>
-      </c>
-      <c r="E43">
-        <v>2.41</v>
-      </c>
-      <c r="F43">
+        <v>1.6622340425531915E-5</v>
+      </c>
+      <c r="C44" s="8">
+        <f t="shared" si="4"/>
+        <v>2.1008403361344539E-4</v>
+      </c>
+      <c r="D44" s="6">
+        <v>30.08</v>
+      </c>
+      <c r="E44" s="6">
+        <v>2.38</v>
+      </c>
+      <c r="F44" s="6">
         <v>582</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G44" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H43" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I43" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J43">
-        <v>886</v>
-      </c>
-      <c r="K43">
+      <c r="H44" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I44" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J44" s="6">
+        <v>886</v>
+      </c>
+      <c r="K44" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L43"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6622340425531915E-5</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="L44" s="10">
+        <v>2.8945154061813598E-19</v>
+      </c>
+      <c r="M44" s="6">
+        <v>2</v>
+      </c>
+      <c r="N44" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8">
         <f t="shared" si="3"/>
-        <v>2.1008403361344539E-4</v>
-      </c>
-      <c r="D44">
-        <v>30.08</v>
-      </c>
-      <c r="E44">
-        <v>2.38</v>
-      </c>
-      <c r="F44">
+        <v>1.7674089784376105E-5</v>
+      </c>
+      <c r="C45" s="8">
+        <f t="shared" si="4"/>
+        <v>1.0351966873706004E-4</v>
+      </c>
+      <c r="D45" s="6">
+        <v>28.29</v>
+      </c>
+      <c r="E45" s="6">
+        <v>4.83</v>
+      </c>
+      <c r="F45" s="6">
         <v>582</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G45" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H44" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I44" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J44">
-        <v>886</v>
-      </c>
-      <c r="K44">
+      <c r="H45" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I45" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J45" s="6">
+        <v>886</v>
+      </c>
+      <c r="K45" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L44">
-        <v>2.8945154061813598E-19</v>
-      </c>
-      <c r="M44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1">
-        <f t="shared" si="2"/>
-        <v>1.7674089784376105E-5</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="L45" s="10">
+        <v>1.611410157598895E-19</v>
+      </c>
+      <c r="M45" s="6">
+        <v>1</v>
+      </c>
+      <c r="N45" s="8">
+        <f t="shared" si="0"/>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8">
         <f t="shared" si="3"/>
-        <v>1.0351966873706004E-4</v>
-      </c>
-      <c r="D45">
-        <v>28.29</v>
-      </c>
-      <c r="E45">
-        <v>4.83</v>
-      </c>
-      <c r="F45">
-        <v>582</v>
-      </c>
-      <c r="G45" s="1">
+        <v>7.8210542781166897E-6</v>
+      </c>
+      <c r="C46" s="8">
+        <f t="shared" si="4"/>
+        <v>3.0120481927710846E-4</v>
+      </c>
+      <c r="D46" s="6">
+        <v>63.93</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1.66</v>
+      </c>
+      <c r="F46" s="6">
+        <v>583</v>
+      </c>
+      <c r="G46" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H45" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I45" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J45">
-        <v>886</v>
-      </c>
-      <c r="K45">
+      <c r="H46" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I46" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J46" s="6">
+        <v>886</v>
+      </c>
+      <c r="K46" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L45">
-        <v>1.611410157598895E-19</v>
-      </c>
-      <c r="M45">
+      <c r="M46" s="6"/>
+      <c r="N46" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8">
+        <f t="shared" si="3"/>
+        <v>7.9567154678548696E-6</v>
+      </c>
+      <c r="C47" s="8">
+        <f t="shared" si="4"/>
+        <v>2.136752136752137E-4</v>
+      </c>
+      <c r="D47" s="6">
+        <v>62.84</v>
+      </c>
+      <c r="E47" s="6">
+        <v>2.34</v>
+      </c>
+      <c r="F47" s="6">
+        <v>583</v>
+      </c>
+      <c r="G47" s="8">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H47" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I47" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J47" s="6">
+        <v>886</v>
+      </c>
+      <c r="K47" s="6">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="L47" s="10">
+        <v>1.690280283048925E-19</v>
+      </c>
+      <c r="M47" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1">
-        <f t="shared" si="2"/>
-        <v>7.8210542781166897E-6</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="N47" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8">
         <f t="shared" si="3"/>
-        <v>3.0120481927710846E-4</v>
-      </c>
-      <c r="D46">
-        <v>63.93</v>
-      </c>
-      <c r="E46">
-        <v>1.66</v>
-      </c>
-      <c r="F46">
+        <v>8.0606158310494929E-6</v>
+      </c>
+      <c r="C48" s="8">
+        <f t="shared" si="4"/>
+        <v>6.0240963855421692E-4</v>
+      </c>
+      <c r="D48" s="6">
+        <v>62.03</v>
+      </c>
+      <c r="E48" s="6">
+        <v>0.83</v>
+      </c>
+      <c r="F48" s="6">
         <v>583</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G48" s="8">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H46" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I46" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J46">
-        <v>886</v>
-      </c>
-      <c r="K46">
+      <c r="H48" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I48" s="8">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J48" s="6">
+        <v>886</v>
+      </c>
+      <c r="K48" s="6">
         <v>94472.244000000006</v>
       </c>
-      <c r="L46"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1">
-        <f t="shared" si="2"/>
-        <v>7.9567154678548696E-6</v>
-      </c>
-      <c r="C47" s="1">
-        <f t="shared" si="3"/>
-        <v>2.136752136752137E-4</v>
-      </c>
-      <c r="D47">
-        <v>62.84</v>
-      </c>
-      <c r="E47">
-        <v>2.34</v>
-      </c>
-      <c r="F47">
-        <v>583</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H47" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I47" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J47">
-        <v>886</v>
-      </c>
-      <c r="K47">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L47">
-        <v>1.690280283048925E-19</v>
-      </c>
-      <c r="M47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1">
-        <f t="shared" si="2"/>
-        <v>8.0606158310494929E-6</v>
-      </c>
-      <c r="C48" s="1">
-        <f t="shared" si="3"/>
-        <v>6.0240963855421692E-4</v>
-      </c>
-      <c r="D48">
-        <v>62.03</v>
-      </c>
-      <c r="E48">
-        <v>0.83</v>
-      </c>
-      <c r="F48">
-        <v>583</v>
-      </c>
-      <c r="G48" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H48" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I48" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J48">
-        <v>886</v>
-      </c>
-      <c r="K48">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L48">
+      <c r="L48" s="10">
         <v>4.7003150270511174E-19</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="L49" s="8">
+      <c r="N48" s="8">
+        <f t="shared" si="0"/>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A49" s="6"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="6"/>
+      <c r="L49" s="10">
         <f>SUM(L2:L48)</f>
         <v>9.3129085708425031E-18</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="6">
         <f>SUM(M2:M48)</f>
         <v>60</v>
       </c>
-      <c r="N49" t="s">
+      <c r="N49" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O49" t="s">
+      <c r="O49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="6">
         <f>L49/M49</f>
         <v>1.5521514284737505E-19</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="O50" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A50" s="6"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="6">
         <f>1.602176634E-19-P49</f>
         <v>5.0025205526249379E-21</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="O51" s="13" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A51" s="6"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P51" s="14">
+      <c r="P51" s="12">
         <f>P50/P49</f>
         <v>3.2229590881760667E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="H53" s="1"/>
@@ -3905,4 +4220,187 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67644AD2-B82B-4CF0-B85E-F3756A511C5B}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="4" width="21.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13">
+        <f>SUM(Tabelle1!N2:N48)/COUNT(Tabelle1!N2:N48)</f>
+        <v>76749.720044792892</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:D10" si="0">C2/B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="13">
+        <f>SUM(Tabelle1!E2:E48)/COUNT(Tabelle1!E2:E48)</f>
+        <v>3.7861702127659589</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="13">
+        <f>SUM(Tabelle1!D2:D48)/COUNT(Tabelle1!D2:D48)</f>
+        <v>32.579148936170206</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="13">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13">
+        <f>SUM(Tabelle1!C2:C48)/COUNT(Tabelle1!C2:C48)</f>
+        <v>2.2029184718617203E-4</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="13">
+        <f>SUM(Tabelle1!B2:B48)/COUNT(Tabelle1!B2:B48)</f>
+        <v>1.7746347463415928E-5</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13">
+        <f>SUM(Tabelle1!K2:K48)/COUNT(Tabelle1!K2:K48)</f>
+        <v>94410.061276595719</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0592091419899335E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="13">
+        <f>SUM(Tabelle1!G2:G48)/COUNT(Tabelle1!G2:G48)</f>
+        <v>1.8184255319148945E-5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4992628647649332E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="13">
+        <v>886</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6433408577878104E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="13">
+        <v>9.81</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <f>C11/B11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="C12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D12" s="4">
+        <f>C12/B12</f>
+        <v>1.2195121951219512E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Durchführung angefangen Vorbereitungen fertig
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/samuel_egli_ksbg_ch/Documents/1/4. Kanti/Maturaarbeit/Arbeit/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A64FF50C-4A65-4BC0-A464-389E9324E554}"/>
+  <xr:revisionPtr revIDLastSave="310" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB228A47-D38D-4A2A-A955-EDD30AFE9F5A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Tröpfchen</t>
   </si>
@@ -134,6 +134,12 @@
   <si>
     <t>elektrischesFeld</t>
   </si>
+  <si>
+    <t>vernachlässigbar</t>
+  </si>
+  <si>
+    <t>allgemeiner Fehler für die Ladung</t>
+  </si>
 </sst>
 </file>
 
@@ -142,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,25 +206,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -339,7 +338,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="15875">
+              <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -347,6 +346,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="2.900000000000003E-20"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$A$2:$A$48</c:f>
@@ -1838,64 +1857,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="65" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P82" sqref="P82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="20.73046875" customWidth="1"/>
-    <col min="11" max="11" width="20.73046875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="20.73046875" style="10" customWidth="1"/>
-    <col min="13" max="14" width="20.73046875" customWidth="1"/>
-    <col min="16" max="16" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="14" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="O1"/>
+      <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
       <c r="S1"/>
@@ -1908,377 +1924,362 @@
       <c r="Z1"/>
       <c r="AA1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A2" s="6">
+    <row r="2" spans="1:27">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="1">
         <v>2.11954217888936E-5</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="1">
         <v>2.0080321285139999E-4</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2">
         <v>23.59</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2">
         <v>585</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H2" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I2" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J2" s="6">
-        <v>886</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="H2" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J2">
+        <v>886</v>
+      </c>
+      <c r="K2">
         <v>94364</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2">
         <v>3.2747980958213941E-19</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="1">
         <f>F2/H2</f>
         <v>76973.68421052632</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="1">
         <v>2.158894645941278E-5</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="1">
         <v>8.4602368866328257E-5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3">
         <v>23.16</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
         <v>5.91</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3">
         <v>585</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H3" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I3" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J3" s="6">
-        <v>886</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="H3" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J3">
+        <v>886</v>
+      </c>
+      <c r="K3">
         <v>94364</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3">
         <v>1.5851685892692281E-19</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="1">
         <f t="shared" ref="N3:N48" si="0">F3/H3</f>
         <v>76973.68421052632</v>
       </c>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A4" s="6">
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="1">
         <v>1.9833399444664819E-5</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="1">
         <v>8.6805555555555559E-5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>25.21</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4">
         <v>5.76</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4">
         <v>585</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H4" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I4" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J4" s="6">
-        <v>886</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="H4" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J4">
+        <v>886</v>
+      </c>
+      <c r="K4">
         <v>94364</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4">
         <v>1.5068138364557E-19</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A5" s="6">
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="1">
         <v>2.4715768660405332E-5</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="1">
         <v>9.3808630393996234E-5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>20.23</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5">
         <v>5.33</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5">
         <v>585</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H5" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I5" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J5" s="6">
-        <v>886</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="H5" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J5">
+        <v>886</v>
+      </c>
+      <c r="K5">
         <v>94364</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="8">
+      <c r="N5" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A6" s="6">
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="1">
         <v>2.04164965291956E-5</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="1">
         <f>0.0005/E6</f>
         <v>8.9126559714795006E-5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>24.49</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6">
         <v>5.61</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>585</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H6" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I6" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J6" s="6">
-        <v>886</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="H6" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J6">
+        <v>886</v>
+      </c>
+      <c r="K6">
         <v>94364</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6">
         <v>1.5772476256952349E-19</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A7" s="6">
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="1">
         <v>1.975503753457132E-5</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="1">
         <v>1.9685039370070001E-4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>25.31</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7">
         <v>2.54</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
         <v>585</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H7" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I7" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J7" s="6">
-        <v>886</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="H7" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J7">
+        <v>886</v>
+      </c>
+      <c r="K7">
         <v>94364</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7">
         <v>3.052773302419662E-19</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7">
         <v>2</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A8" s="6">
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="1">
         <v>2.044153720359771E-5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="1">
         <v>1.97628458498E-4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>24.46</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8">
         <v>2.5299999999999998</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
         <v>585</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H8" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I8" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J8" s="6">
-        <v>886</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="H8" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J8">
+        <v>886</v>
+      </c>
+      <c r="K8">
         <v>94364</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8">
         <v>3.1423605559845701E-19</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8">
         <v>2</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6">
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="1">
         <v>1.8429782528566169E-5</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="1">
         <v>9.328358208955224E-5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>27.13</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9">
         <v>5.36</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9">
         <v>585</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="6">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H9" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I9" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J9" s="6">
-        <v>886</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="H9" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J9">
+        <v>886</v>
+      </c>
+      <c r="K9">
         <v>94364</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9">
         <v>1.5046225734477661E-19</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>76973.68421052632</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
@@ -2291,324 +2292,310 @@
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A10" s="6">
+    <row r="10" spans="1:27">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="1">
         <v>1.708817498291182E-5</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="1">
         <v>1.2562814070350001E-4</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>29.26</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10">
         <v>3.98</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10">
         <v>586</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H10" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I10" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J10" s="6">
-        <v>886</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="H10" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J10">
+        <v>886</v>
+      </c>
+      <c r="K10">
         <v>94364</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10">
         <v>1.8492070982804951E-19</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10">
         <v>1</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A11" s="6">
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="1">
         <v>1.692620176032498E-5</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="1">
         <v>3.9062500000000002E-4</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>29.54</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11">
         <v>1.28</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11">
         <v>586</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H11" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I11" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J11" s="6">
-        <v>886</v>
-      </c>
-      <c r="K11" s="6">
+      <c r="H11" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J11">
+        <v>886</v>
+      </c>
+      <c r="K11">
         <v>94364</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="8">
+      <c r="N11" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A12" s="6">
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="1">
         <v>1.2333497779970399E-5</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="1">
         <v>1.121076233183E-4</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12">
         <v>40.54</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12">
         <v>4.46</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12">
         <v>586</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H12" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I12" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J12" s="6">
-        <v>886</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="H12" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I12" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J12">
+        <v>886</v>
+      </c>
+      <c r="K12">
         <v>94364</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12">
         <v>1.2938659935743371E-19</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A13" s="6">
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="1">
         <v>1.289324394017535E-5</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="1">
         <v>1.295336787564E-4</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13">
         <v>38.78</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13">
         <v>3.86</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13">
         <v>586</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H13" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I13" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J13" s="6">
-        <v>886</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="H13" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J13">
+        <v>886</v>
+      </c>
+      <c r="K13">
         <v>94364</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13">
         <v>1.5267483032452281E-19</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A14" s="6">
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="1">
         <v>1.316135825217162E-5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="1">
         <v>2.2624434389139999E-4</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14">
         <v>37.99</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14">
         <v>2.21</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14">
         <v>586</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H14" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I14" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J14" s="6">
-        <v>886</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="H14" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J14">
+        <v>886</v>
+      </c>
+      <c r="K14">
         <v>94364</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="8">
+      <c r="N14" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A15" s="6">
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="1">
         <v>1.151012891344383E-5</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="1">
         <v>1.262626262626E-4</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15">
         <v>43.44</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15">
         <v>3.96</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15">
         <v>586</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H15" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I15" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J15" s="6">
-        <v>886</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="H15" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J15">
+        <v>886</v>
+      </c>
+      <c r="K15">
         <v>94364</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15">
         <v>1.365537769282638E-19</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15">
         <v>1</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="6">
+    </row>
+    <row r="16" spans="1:27" s="2" customFormat="1">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="1">
         <v>1.575299306868305E-5</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="1">
         <v>1.210653753026E-4</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16">
         <v>31.74</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16">
         <v>4.13</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16">
         <v>586</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="6">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H16" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I16" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J16" s="6">
-        <v>886</v>
-      </c>
-      <c r="K16" s="6">
+      <c r="H16" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J16">
+        <v>886</v>
+      </c>
+      <c r="K16">
         <v>94364</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16">
         <v>1.679480167697637E-19</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16">
         <v>1</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="1">
         <f t="shared" si="0"/>
         <v>77105.263157894733</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
+      <c r="O16"/>
+      <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
       <c r="S16"/>
@@ -2621,231 +2608,222 @@
       <c r="Z16"/>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A17" s="6">
+    <row r="17" spans="1:27">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="1">
         <v>1.8109380659181451E-5</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="1">
         <v>2.2624434389139999E-4</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17">
         <v>27.61</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17">
         <v>2.21</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17">
         <v>580</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="6">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H17" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I17" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J17" s="6">
-        <v>886</v>
-      </c>
-      <c r="K17" s="6">
+      <c r="H17" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J17">
+        <v>886</v>
+      </c>
+      <c r="K17">
         <v>94364</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17">
         <v>3.3115626946853271E-19</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17">
         <v>2</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="1">
         <f t="shared" si="0"/>
         <v>76315.789473684214</v>
       </c>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A18" s="6">
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="1">
         <v>1.212709192335678E-5</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="1">
         <v>4.5045045045039999E-4</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>41.23</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18">
         <v>580</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="6">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H18" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I18" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J18" s="6">
-        <v>886</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="H18" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J18">
+        <v>886</v>
+      </c>
+      <c r="K18">
         <v>94364</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18">
         <v>4.7852879920201003E-19</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18">
         <v>3</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="1">
         <f t="shared" si="0"/>
         <v>76315.789473684214</v>
       </c>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A19" s="6">
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="1">
         <v>1.07781849536538E-5</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="1">
         <v>4.5045045045039999E-4</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19">
         <v>46.39</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19">
         <v>580</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="6">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H19" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I19" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J19" s="6">
-        <v>886</v>
-      </c>
-      <c r="K19" s="6">
+      <c r="H19" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I19" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J19">
+        <v>886</v>
+      </c>
+      <c r="K19">
         <v>94364</v>
       </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="8">
+      <c r="N19" s="1">
         <f t="shared" si="0"/>
         <v>76315.789473684214</v>
       </c>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A20" s="6">
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="1">
         <v>1.065189603749468E-5</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="1">
         <v>2.8409090909090002E-4</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20">
         <v>46.94</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20">
         <v>1.76</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20">
         <v>580</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="6">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H20" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I20" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J20" s="6">
-        <v>886</v>
-      </c>
-      <c r="K20" s="6">
+      <c r="H20" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J20">
+        <v>886</v>
+      </c>
+      <c r="K20">
         <v>94364</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20">
         <v>2.7853483615976351E-19</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20">
         <v>2</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="1">
         <f t="shared" si="0"/>
         <v>76315.789473684214</v>
       </c>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="6">
+    </row>
+    <row r="21" spans="1:27" s="2" customFormat="1">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="1">
         <v>1.147842056932966E-5</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="1">
         <v>5.6179775280890002E-4</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21">
         <v>43.56</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21">
         <v>0.89</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21">
         <v>580</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="6">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H21" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I21" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J21" s="6">
-        <v>886</v>
-      </c>
-      <c r="K21" s="6">
+      <c r="H21" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J21">
+        <v>886</v>
+      </c>
+      <c r="K21">
         <v>94364</v>
       </c>
-      <c r="L21" s="10"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="8">
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21" s="1">
         <f t="shared" si="0"/>
         <v>76315.789473684214</v>
       </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="O21"/>
+      <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
@@ -2858,1358 +2836,1277 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A22" s="6">
+    <row r="22" spans="1:27">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="1">
         <v>1.11656989727557E-5</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="1">
         <v>1.179245283018E-4</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22">
         <v>44.78</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22">
         <v>4.24</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22">
         <v>583</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H22" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I22" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J22" s="6">
-        <v>886</v>
-      </c>
-      <c r="K22" s="6">
+      <c r="H22" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I22" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J22">
+        <v>886</v>
+      </c>
+      <c r="K22">
         <v>94364</v>
       </c>
-      <c r="M22" s="6"/>
-      <c r="N22" s="8">
+      <c r="N22" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A23" s="6">
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="1">
         <v>1.4033118158854901E-5</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="1">
         <v>2.427184466019E-4</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23">
         <v>35.630000000000003</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23">
         <v>2.06</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23">
         <v>583</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H23" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I23" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J23" s="6">
-        <v>886</v>
-      </c>
-      <c r="K23" s="6">
+      <c r="H23" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I23" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J23">
+        <v>886</v>
+      </c>
+      <c r="K23">
         <v>94364</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23">
         <v>2.9254518781664188E-19</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23">
         <v>2</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A24" s="6">
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="1">
         <v>1.282380097460887E-5</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="1">
         <v>1.2562814070350001E-4</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24">
         <v>38.99</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24">
         <v>3.98</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24">
         <v>583</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H24" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I24" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J24" s="6">
-        <v>886</v>
-      </c>
-      <c r="K24" s="6">
+      <c r="H24" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J24">
+        <v>886</v>
+      </c>
+      <c r="K24">
         <v>94364</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24">
         <v>1.483515883555309E-19</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24">
         <v>1</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A25" s="6">
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="1">
         <v>1.304461257500652E-5</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="1">
         <v>3.9682539682530001E-4</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25">
         <v>38.33</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25">
         <v>1.26</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25">
         <v>583</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H25" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I25" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J25" s="6">
-        <v>886</v>
-      </c>
-      <c r="K25" s="6">
+      <c r="H25" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I25" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J25">
+        <v>886</v>
+      </c>
+      <c r="K25">
         <v>94364</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25">
         <v>4.4434402544902837E-19</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25">
         <v>3</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A26" s="6">
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="1">
         <v>1.446759259259259E-5</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="1">
         <v>2.4875621890539998E-4</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>34.56</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26">
         <v>583</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H26" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I26" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J26" s="6">
-        <v>886</v>
-      </c>
-      <c r="K26" s="6">
+      <c r="H26" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I26" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J26">
+        <v>886</v>
+      </c>
+      <c r="K26">
         <v>94364</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26">
         <v>3.0617078747401381E-19</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26">
         <v>2</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A27" s="6">
+    </row>
+    <row r="27" spans="1:27">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="1">
         <v>1.032204789430223E-5</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="1">
         <v>2.3923444976069999E-4</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27">
         <v>48.44</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27">
         <v>2.09</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27">
         <v>583</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H27" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I27" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J27" s="6">
-        <v>886</v>
-      </c>
-      <c r="K27" s="6">
+      <c r="H27" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J27">
+        <v>886</v>
+      </c>
+      <c r="K27">
         <v>94364</v>
       </c>
-      <c r="M27" s="6"/>
-      <c r="N27" s="8">
+      <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="6">
+    </row>
+    <row r="28" spans="1:27">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="1">
         <v>1.047339757017176E-5</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="1">
         <v>2.6178010471200001E-4</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28">
         <v>47.74</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28">
         <v>1.91</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28">
         <v>583</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="6">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H28" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I28" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J28" s="6">
-        <v>886</v>
-      </c>
-      <c r="K28" s="6">
+      <c r="H28" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I28" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J28">
+        <v>886</v>
+      </c>
+      <c r="K28">
         <v>94364</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="N28" s="8">
+      <c r="N28" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A29" s="6">
+    <row r="29" spans="1:27">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="1">
         <f>0.0005/D29</f>
         <v>3.6284470246734402E-5</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="1">
         <f>0.0005/E29</f>
         <v>3.048780487804878E-4</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29">
         <v>13.78</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29">
         <v>1.64</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29">
         <v>583</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H29" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I29" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J29" s="6">
-        <v>886</v>
-      </c>
-      <c r="K29" s="6">
+      <c r="H29" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J29">
+        <v>886</v>
+      </c>
+      <c r="K29">
         <v>94472.244000000006</v>
       </c>
-      <c r="M29" s="6"/>
-      <c r="N29" s="8">
+      <c r="N29" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A30" s="6">
+    </row>
+    <row r="30" spans="1:27">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="1">
         <f t="shared" ref="B30:B40" si="1">0.0005/D30</f>
         <v>3.3579583613163193E-5</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="1">
         <f t="shared" ref="C30:C40" si="2">0.0005/E30</f>
         <v>3.95882818685669E-5</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30">
         <v>14.89</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30">
         <v>12.63</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30">
         <v>583</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H30" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I30" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J30" s="6">
-        <v>886</v>
-      </c>
-      <c r="K30" s="6">
+      <c r="H30" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I30" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J30">
+        <v>886</v>
+      </c>
+      <c r="K30">
         <v>94472.244000000006</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30">
         <v>1.4554623175668291E-19</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M30">
         <v>1</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A31" s="6">
+    </row>
+    <row r="31" spans="1:27">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="1">
         <f t="shared" si="1"/>
         <v>1.4744913005013272E-5</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="1">
         <f t="shared" si="2"/>
         <v>1.0438413361169103E-4</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31">
         <v>33.909999999999997</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31">
         <v>4.79</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31">
         <v>583</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H31" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I31" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J31" s="6">
-        <v>886</v>
-      </c>
-      <c r="K31" s="6">
+      <c r="H31" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I31" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J31">
+        <v>886</v>
+      </c>
+      <c r="K31">
         <v>94472.244000000006</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31">
         <v>1.3963446372113281E-19</v>
       </c>
-      <c r="M31" s="6">
+      <c r="M31">
         <v>1</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A32" s="6">
+    </row>
+    <row r="32" spans="1:27">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="1">
         <f t="shared" si="1"/>
         <v>2.8851702250432778E-5</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="1">
         <f t="shared" si="2"/>
         <v>5.2192066805845514E-5</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32">
         <v>17.329999999999998</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32">
         <v>9.58</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32">
         <v>583</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H32" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I32" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J32" s="6">
-        <v>886</v>
-      </c>
-      <c r="K32" s="6">
+      <c r="H32" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I32" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J32">
+        <v>886</v>
+      </c>
+      <c r="K32">
         <v>94472.244000000006</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32">
         <v>1.4673753039611549E-19</v>
       </c>
-      <c r="M32" s="6">
+      <c r="M32">
         <v>1</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A33" s="6">
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="1">
         <f t="shared" si="1"/>
         <v>3.0618493570116355E-5</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="1">
         <f t="shared" si="2"/>
         <v>5.3995680345572353E-5</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33">
         <v>16.329999999999998</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33">
         <v>9.26</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33">
         <v>583</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H33" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I33" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J33" s="6">
-        <v>886</v>
-      </c>
-      <c r="K33" s="6">
+      <c r="H33" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J33">
+        <v>886</v>
+      </c>
+      <c r="K33">
         <v>94472.244000000006</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33">
         <v>1.5897872941404839E-19</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33">
         <v>1</v>
       </c>
-      <c r="N33" s="8">
+      <c r="N33" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A34" s="6">
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="1">
         <f t="shared" si="1"/>
         <v>2.6695141484249868E-5</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="1">
         <f t="shared" si="2"/>
         <v>5.8207217694994179E-5</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34">
         <v>18.73</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34">
         <v>8.59</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34">
         <v>583</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H34" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I34" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J34" s="6">
-        <v>886</v>
-      </c>
-      <c r="K34" s="6">
+      <c r="H34" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I34" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J34">
+        <v>886</v>
+      </c>
+      <c r="K34">
         <v>94472.244000000006</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34">
         <v>1.4641553540058561E-19</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34">
         <v>1</v>
       </c>
-      <c r="N34" s="8">
+      <c r="N34" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A35" s="6">
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="1">
         <f t="shared" si="1"/>
         <v>2.9779630732578919E-5</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="1">
         <f t="shared" si="2"/>
         <v>5.3418803418803426E-5</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35">
         <v>16.79</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35">
         <v>9.36</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35">
         <v>583</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H35" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I35" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J35" s="6">
-        <v>886</v>
-      </c>
-      <c r="K35" s="6">
+      <c r="H35" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I35" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J35">
+        <v>886</v>
+      </c>
+      <c r="K35">
         <v>94472.244000000006</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35">
         <v>1.536419009789623E-19</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35">
         <v>1</v>
       </c>
-      <c r="N35" s="8">
+      <c r="N35" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A36" s="6">
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="1">
         <f t="shared" si="1"/>
         <v>2.7917364600781685E-5</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="1">
         <f t="shared" si="2"/>
         <v>5.76036866359447E-5</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36">
         <v>17.91</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36">
         <v>8.68</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36">
         <v>583</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H36" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I36" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J36" s="6">
-        <v>886</v>
-      </c>
-      <c r="K36" s="6">
+      <c r="H36" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I36" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J36">
+        <v>886</v>
+      </c>
+      <c r="K36">
         <v>94472.244000000006</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36">
         <v>1.5168780241725071E-19</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36">
         <v>1</v>
       </c>
-      <c r="N36" s="8">
+      <c r="N36" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A37" s="6">
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="1">
         <f t="shared" si="1"/>
         <v>3.0138637733574443E-5</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="1">
         <f t="shared" si="2"/>
         <v>5.8072009291521493E-5</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37">
         <v>16.59</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37">
         <v>8.61</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37">
         <v>583</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="6">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H37" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I37" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J37" s="6">
-        <v>886</v>
-      </c>
-      <c r="K37" s="6">
+      <c r="H37" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I37" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J37">
+        <v>886</v>
+      </c>
+      <c r="K37">
         <v>94472.244000000006</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L37">
         <v>1.641171292859742E-19</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37">
         <v>1</v>
       </c>
-      <c r="N37" s="8">
+      <c r="N37" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A38" s="6">
+    <row r="38" spans="1:17">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="1">
         <f t="shared" si="1"/>
         <v>1.8946570670708603E-5</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="1">
         <f t="shared" si="2"/>
         <v>5.3191489361702129E-4</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38">
         <v>26.39</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38">
         <v>0.94</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38">
         <v>582</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H38" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I38" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J38" s="6">
-        <v>886</v>
-      </c>
-      <c r="K38" s="6">
+      <c r="H38" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I38" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J38">
+        <v>886</v>
+      </c>
+      <c r="K38">
         <v>94472.244000000006</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38">
         <v>7.6660747025858679E-19</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38">
         <v>5</v>
       </c>
-      <c r="N38" s="8">
+      <c r="N38" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A39" s="6">
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="1">
         <f t="shared" si="1"/>
         <v>1.8982536066818528E-5</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="1">
         <f t="shared" si="2"/>
         <v>3.5460992907801421E-4</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39">
         <v>26.34</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39">
         <v>1.41</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39">
         <v>582</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H39" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I39" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J39" s="6">
-        <v>886</v>
-      </c>
-      <c r="K39" s="6">
+      <c r="H39" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I39" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J39">
+        <v>886</v>
+      </c>
+      <c r="K39">
         <v>94472.244000000006</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39">
         <v>5.2055514577343985E-19</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M39">
         <v>3</v>
       </c>
-      <c r="N39" s="8">
+      <c r="N39" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A40" s="6">
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="1">
         <f t="shared" si="1"/>
         <v>1.6539861065167053E-5</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="1">
         <f t="shared" si="2"/>
         <v>3.3112582781456954E-4</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40">
         <v>30.23</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40">
         <v>1.51</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40">
         <v>582</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H40" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I40" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J40" s="6">
-        <v>886</v>
-      </c>
-      <c r="K40" s="6">
+      <c r="H40" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I40" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J40">
+        <v>886</v>
+      </c>
+      <c r="K40">
         <v>94472.244000000006</v>
       </c>
-      <c r="L40" s="10">
+      <c r="L40">
         <v>4.4242549593716838E-19</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40">
         <v>3</v>
       </c>
-      <c r="N40" s="8">
+      <c r="N40" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A41" s="6">
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="1">
         <f>0.0005/D41</f>
         <v>1.7768301350390903E-5</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="1">
         <f>0.0005/E41</f>
         <v>4.8543689320388347E-4</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41">
         <v>28.14</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41">
         <v>1.03</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41">
         <v>582</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H41" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I41" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J41" s="6">
-        <v>886</v>
-      </c>
-      <c r="K41" s="6">
+      <c r="H41" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I41" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J41">
+        <v>886</v>
+      </c>
+      <c r="K41">
         <v>94472.244000000006</v>
       </c>
-      <c r="L41" s="10">
+      <c r="L41">
         <v>6.7141516307161576E-19</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41">
         <v>4</v>
       </c>
-      <c r="N41" s="8">
+      <c r="N41" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A42" s="6">
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="1">
         <f t="shared" ref="B42:B48" si="3">0.0005/D42</f>
         <v>1.4667057788207684E-5</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="1">
         <f t="shared" ref="C42:C48" si="4">0.0005/E42</f>
         <v>3.4965034965034965E-4</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42">
         <v>34.090000000000003</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42">
         <v>1.43</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42">
         <v>582</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H42" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I42" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J42" s="6">
-        <v>886</v>
-      </c>
-      <c r="K42" s="6">
+      <c r="H42" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I42" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J42">
+        <v>886</v>
+      </c>
+      <c r="K42">
         <v>94472.244000000006</v>
       </c>
-      <c r="M42" s="6"/>
-      <c r="N42" s="8">
+      <c r="N42" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A43" s="6">
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="1">
         <f t="shared" si="3"/>
         <v>1.4912019087384431E-5</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="1">
         <f t="shared" si="4"/>
         <v>2.0746887966804979E-4</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43">
         <v>33.53</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43">
         <v>2.41</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43">
         <v>582</v>
       </c>
-      <c r="G43" s="8">
+      <c r="G43" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H43" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I43" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J43" s="6">
-        <v>886</v>
-      </c>
-      <c r="K43" s="6">
+      <c r="H43" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I43" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J43">
+        <v>886</v>
+      </c>
+      <c r="K43">
         <v>94472.244000000006</v>
       </c>
-      <c r="M43" s="6"/>
-      <c r="N43" s="8">
+      <c r="N43" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A44" s="6">
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="1">
         <f t="shared" si="3"/>
         <v>1.6622340425531915E-5</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="1">
         <f t="shared" si="4"/>
         <v>2.1008403361344539E-4</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44">
         <v>30.08</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44">
         <v>2.38</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44">
         <v>582</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H44" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I44" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J44" s="6">
-        <v>886</v>
-      </c>
-      <c r="K44" s="6">
+      <c r="H44" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I44" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J44">
+        <v>886</v>
+      </c>
+      <c r="K44">
         <v>94472.244000000006</v>
       </c>
-      <c r="L44" s="10">
+      <c r="L44">
         <v>2.8945154061813598E-19</v>
       </c>
-      <c r="M44" s="6">
+      <c r="M44">
         <v>2</v>
       </c>
-      <c r="N44" s="8">
+      <c r="N44" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A45" s="6">
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="1">
         <f t="shared" si="3"/>
         <v>1.7674089784376105E-5</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="1">
         <f t="shared" si="4"/>
         <v>1.0351966873706004E-4</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45">
         <v>28.29</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45">
         <v>4.83</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45">
         <v>582</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H45" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I45" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J45" s="6">
-        <v>886</v>
-      </c>
-      <c r="K45" s="6">
+      <c r="H45" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I45" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J45">
+        <v>886</v>
+      </c>
+      <c r="K45">
         <v>94472.244000000006</v>
       </c>
-      <c r="L45" s="10">
+      <c r="L45">
         <v>1.611410157598895E-19</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45">
         <v>1</v>
       </c>
-      <c r="N45" s="8">
+      <c r="N45" s="1">
         <f t="shared" si="0"/>
         <v>76578.947368421053</v>
       </c>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A46" s="6">
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="1">
         <f t="shared" si="3"/>
         <v>7.8210542781166897E-6</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="1">
         <f t="shared" si="4"/>
         <v>3.0120481927710846E-4</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46">
         <v>63.93</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46">
         <v>1.66</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46">
         <v>583</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H46" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I46" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J46" s="6">
-        <v>886</v>
-      </c>
-      <c r="K46" s="6">
+      <c r="H46" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I46" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J46">
+        <v>886</v>
+      </c>
+      <c r="K46">
         <v>94472.244000000006</v>
       </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="8">
+      <c r="N46" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A47" s="6">
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="1">
         <f t="shared" si="3"/>
         <v>7.9567154678548696E-6</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="1">
         <f t="shared" si="4"/>
         <v>2.136752136752137E-4</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47">
         <v>62.84</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47">
         <v>2.34</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47">
         <v>583</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H47" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I47" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J47" s="6">
-        <v>886</v>
-      </c>
-      <c r="K47" s="6">
+      <c r="H47" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I47" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J47">
+        <v>886</v>
+      </c>
+      <c r="K47">
         <v>94472.244000000006</v>
       </c>
-      <c r="L47" s="10">
+      <c r="L47">
         <v>1.690280283048925E-19</v>
       </c>
-      <c r="M47" s="6">
+      <c r="M47">
         <v>1</v>
       </c>
-      <c r="N47" s="8">
+      <c r="N47" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A48" s="6">
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="1">
         <f t="shared" si="3"/>
         <v>8.0606158310494929E-6</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="1">
         <f t="shared" si="4"/>
         <v>6.0240963855421692E-4</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48">
         <v>62.03</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48">
         <v>0.83</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48">
         <v>583</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="1">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H48" s="8">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I48" s="8">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J48" s="6">
-        <v>886</v>
-      </c>
-      <c r="K48" s="6">
+      <c r="H48" s="1">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I48" s="1">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J48">
+        <v>886</v>
+      </c>
+      <c r="K48">
         <v>94472.244000000006</v>
       </c>
-      <c r="L48" s="10">
+      <c r="L48">
         <v>4.7003150270511174E-19</v>
       </c>
-      <c r="M48" s="6">
+      <c r="M48">
         <v>3</v>
       </c>
-      <c r="N48" s="8">
+      <c r="N48" s="1">
         <f t="shared" si="0"/>
         <v>76710.526315789481</v>
       </c>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="6"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="6"/>
-      <c r="L49" s="10">
+    </row>
+    <row r="49" spans="2:16">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="L49">
         <f>SUM(L2:L48)</f>
         <v>9.3129085708425031E-18</v>
       </c>
-      <c r="M49" s="6">
+      <c r="M49">
         <f>SUM(M2:M48)</f>
         <v>60</v>
       </c>
-      <c r="N49" s="6" t="s">
+      <c r="N49" t="s">
         <v>13</v>
       </c>
-      <c r="O49" s="6" t="s">
+      <c r="O49" t="s">
         <v>14</v>
       </c>
-      <c r="P49" s="6">
+      <c r="P49">
         <f>L49/M49</f>
         <v>1.5521514284737505E-19</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A50" s="6"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6" t="s">
+    <row r="50" spans="2:16">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="O50" t="s">
         <v>15</v>
       </c>
-      <c r="P50" s="6">
+      <c r="P50">
         <f>1.602176634E-19-P49</f>
         <v>5.0025205526249379E-21</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A51" s="6"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="11" t="s">
+    <row r="51" spans="2:16">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="O51" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="P51" s="12">
+      <c r="P51" s="8">
         <f>P50/P49</f>
         <v>3.2229590881760667E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:16">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:16">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="H53" s="1"/>
@@ -4224,18 +4121,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67644AD2-B82B-4CF0-B85E-F3756A511C5B}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="21.59765625" customWidth="1"/>
+    <col min="1" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>28</v>
       </c>
@@ -4246,88 +4144,90 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2">
         <f>SUM(Tabelle1!N2:N48)/COUNT(Tabelle1!N2:N48)</f>
         <v>76749.720044792892</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D10" si="0">C2/B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3">
         <f>SUM(Tabelle1!E2:E48)/COUNT(Tabelle1!E2:E48)</f>
         <v>3.7861702127659589</v>
       </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
       <c r="D3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" ref="D3:D10" si="0">C3/B3</f>
+        <v>2.6411913458836745E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4">
         <f>SUM(Tabelle1!D2:D48)/COUNT(Tabelle1!D2:D48)</f>
         <v>32.579148936170206</v>
       </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>3.0694478912239921E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
         <v>5.0000000000000001E-4</v>
       </c>
+      <c r="C5">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="13">
-        <f>SUM(Tabelle1!C2:C48)/COUNT(Tabelle1!C2:C48)</f>
-        <v>2.2029184718617203E-4</v>
-      </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4.6399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="13">
-        <f>SUM(Tabelle1!B2:B48)/COUNT(Tabelle1!B2:B48)</f>
-        <v>1.7746347463415928E-5</v>
+      <c r="B7">
+        <f>B5/B4</f>
+        <v>1.5347239456119959E-5</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2.3099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8">
         <f>SUM(Tabelle1!K2:K48)/COUNT(Tabelle1!K2:K48)</f>
         <v>94410.061276595719</v>
       </c>
@@ -4339,42 +4239,42 @@
         <v>1.0592091419899335E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9">
         <f>SUM(Tabelle1!G2:G48)/COUNT(Tabelle1!G2:G48)</f>
         <v>1.8184255319148945E-5</v>
       </c>
       <c r="C9" s="1">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-8</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>5.4992628647649332E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5.499262864764933E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10">
         <v>886</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>5.6433408577878104E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1.1286681715575621E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11">
         <v>9.81</v>
       </c>
       <c r="C11">
@@ -4384,12 +4284,15 @@
         <f>C11/B11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12">
         <v>8.2000000000000007E-3</v>
       </c>
       <c r="C12">
@@ -4400,7 +4303,16 @@
         <v>1.2195121951219512E-3</v>
       </c>
     </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.18429999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Erster Abschnitt im Kapitel Auswertung fertig. Nächstes das Ergebnis
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/samuel_egli_ksbg_ch/Documents/1/4. Kanti/Maturaarbeit/Arbeit/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="310" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB228A47-D38D-4A2A-A955-EDD30AFE9F5A}"/>
+  <xr:revisionPtr revIDLastSave="316" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3671FE54-2AD6-4F7A-9A24-7973918B8340}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,6 +634,688 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5B70-4590-9803-3CA864082047}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1722374848"/>
+        <c:axId val="1722380608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1722374848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Nummerierung der Tröpfchen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1722380608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1722380608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.000000000000001E-18"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Ladung in Coulomb [C]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1722374848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.6020000000000019E-19"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ladungsdiagramm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ladung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$2:$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="47"/>
+                <c:pt idx="0">
+                  <c:v>3.2747980958213941E-19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5851685892692281E-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5068138364557E-19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5772476256952349E-19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.052773302419662E-19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1423605559845701E-19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5046225734477661E-19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8492070982804951E-19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2938659935743371E-19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5267483032452281E-19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.365537769282638E-19</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.679480167697637E-19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3115626946853271E-19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7852879920201003E-19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7853483615976351E-19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.9254518781664188E-19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.483515883555309E-19</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.4434402544902837E-19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.0617078747401381E-19</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4554623175668291E-19</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3963446372113281E-19</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4673753039611549E-19</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5897872941404839E-19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.4641553540058561E-19</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.536419009789623E-19</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5168780241725071E-19</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.641171292859742E-19</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.6660747025858679E-19</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.2055514577343985E-19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.4242549593716838E-19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.7141516307161576E-19</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.8945154061813598E-19</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.611410157598895E-19</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.690280283048925E-19</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7003150270511174E-19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42B1-4C6A-82BA-7EFE4E62B2C0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -977,7 +1659,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1526,6 +2764,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>862854</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>705971</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>56028</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E9EBCCA-4CCB-433D-9E04-5695A4571C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1857,17 +3133,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P82" sqref="P82"/>
+    <sheetView tabSelected="1" topLeftCell="G59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V100" sqref="V100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="14" width="20.7109375" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1924,7 +3200,7 @@
       <c r="Z1"/>
       <c r="AA1"/>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1969,7 +3245,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2014,7 +3290,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2059,7 +3335,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2098,7 +3374,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2144,7 +3420,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2189,7 +3465,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2234,7 +3510,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="2" customFormat="1">
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2292,7 +3568,7 @@
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2337,7 +3613,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2376,7 +3652,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2421,7 +3697,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2466,7 +3742,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2505,7 +3781,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2550,7 +3826,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="2" customFormat="1">
+    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2608,7 +3884,7 @@
       <c r="Z16"/>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2653,7 +3929,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2698,7 +3974,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2737,7 +4013,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2782,7 +4058,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="2" customFormat="1">
+    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2836,7 +4112,7 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2875,7 +4151,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2920,7 +4196,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2965,7 +4241,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3010,7 +4286,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3055,7 +4331,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3094,7 +4370,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3133,7 +4409,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3174,7 +4450,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3221,7 +4497,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3268,7 +4544,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3315,7 +4591,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3362,7 +4638,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3409,7 +4685,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3456,7 +4732,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3503,7 +4779,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3551,7 +4827,7 @@
       </c>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3598,7 +4874,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3645,7 +4921,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3692,7 +4968,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3739,7 +5015,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3780,7 +5056,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3821,7 +5097,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3868,7 +5144,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3915,7 +5191,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3956,7 +5232,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4003,7 +5279,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4050,7 +5326,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="H49" s="1"/>
@@ -4074,7 +5350,7 @@
         <v>1.5521514284737505E-19</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="H50" s="1"/>
@@ -4087,7 +5363,7 @@
         <v>5.0025205526249379E-21</v>
       </c>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="H51" s="1"/>
@@ -4100,13 +5376,13 @@
         <v>3.2229590881760667E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="H53" s="1"/>
@@ -4123,17 +5399,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67644AD2-B82B-4CF0-B85E-F3756A511C5B}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>28</v>
       </c>
@@ -4144,7 +5420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4156,7 +5432,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4172,7 +5448,7 @@
         <v>2.6411913458836745E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4188,7 +5464,7 @@
         <v>3.0694478912239921E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4203,7 +5479,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4211,7 +5487,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4223,7 +5499,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4239,7 +5515,7 @@
         <v>1.0592091419899335E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -4255,7 +5531,7 @@
         <v>5.499262864764933E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4270,7 +5546,7 @@
         <v>1.1286681715575621E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -4288,7 +5564,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -4303,7 +5579,7 @@
         <v>1.2195121951219512E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Fehlerrechnungunterabschnitt angefangen, Fehlerrechnungstabelle verbessert
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/samuel_egli_ksbg_ch/Documents/1/4. Kanti/Maturaarbeit/Arbeit/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="316" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3671FE54-2AD6-4F7A-9A24-7973918B8340}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E993414-13E0-4059-B91D-37BBBDC38888}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Tröpfchen</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>elektrischesFeld</t>
-  </si>
-  <si>
-    <t>vernachlässigbar</t>
   </si>
   <si>
     <t>allgemeiner Fehler für die Ladung</t>
@@ -3133,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V100" sqref="V100"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,10 +5394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67644AD2-B82B-4CF0-B85E-F3756A511C5B}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,7 +5406,7 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>28</v>
       </c>
@@ -5420,51 +5417,52 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2">
-        <f>SUM(Tabelle1!N2:N48)/COUNT(Tabelle1!N2:N48)</f>
-        <v>76749.720044792892</v>
+        <v>76000</v>
+      </c>
+      <c r="C2">
+        <v>520</v>
       </c>
       <c r="D2" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <f>C2/B2</f>
+        <v>6.842105263157895E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3">
-        <f>SUM(Tabelle1!E2:E48)/COUNT(Tabelle1!E2:E48)</f>
-        <v>3.7861702127659589</v>
+        <v>3.7</v>
       </c>
       <c r="C3">
         <v>0.1</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D10" si="0">C3/B3</f>
-        <v>2.6411913458836745E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.7027027027027029E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4">
-        <f>SUM(Tabelle1!D2:D48)/COUNT(Tabelle1!D2:D48)</f>
-        <v>32.579148936170206</v>
+        <v>32.6</v>
       </c>
       <c r="C4">
         <v>0.1</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>3.0694478912239921E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.0674846625766872E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5479,43 +5477,38 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4">
-        <v>4.6399999999999997E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
-        <f>B5/B4</f>
-        <v>1.5347239456119959E-5</v>
-      </c>
       <c r="D7" s="4">
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8">
-        <f>SUM(Tabelle1!K2:K48)/COUNT(Tabelle1!K2:K48)</f>
-        <v>94410.061276595719</v>
+        <v>94000</v>
       </c>
       <c r="C8">
         <v>1000</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>1.0592091419899335E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0638297872340425E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -5531,7 +5524,7 @@
         <v>5.499262864764933E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -5539,14 +5532,14 @@
         <v>886</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>1.1286681715575621E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.128668171557562E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5560,11 +5553,8 @@
         <f>C11/B11</f>
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5579,9 +5569,9 @@
         <v>1.2195121951219512E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4">
         <v>0.18429999999999999</v>

</xml_diff>

<commit_message>
Fehlerrechnung hinzugefügt, Kapitel Auswertung ist fertig
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bldsg-my.sharepoint.com/personal/samuel_egli_ksbg_ch/Documents/1/4. Kanti/Maturaarbeit/Arbeit/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E993414-13E0-4059-B91D-37BBBDC38888}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{6E283396-03A3-4AEA-B7F6-734CF0FF3341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6785E39-D32E-4E25-93CC-42B11C1228C3}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="2.900000000000003E-20"/>
+            <c:val val="2.1530000000000025E-20"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2733,15 +2733,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>503842</xdr:colOff>
+      <xdr:colOff>503843</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>102978</xdr:rowOff>
+      <xdr:rowOff>102979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1182415</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>98533</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1356276</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>51765</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3130,17 +3130,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="14" width="20.7109375" customWidth="1"/>
+    <col min="1" max="14" width="20.73046875" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="Z1"/>
       <c r="AA1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>76973.68421052632</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3565,7 +3565,7 @@
       <c r="Z9"/>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>77105.263157894733</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="Z16"/>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>76315.789473684214</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4109,7 +4109,7 @@
       <c r="Z21"/>
       <c r="AA21"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4824,7 +4824,7 @@
       </c>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>76578.947368421053</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>76710.526315789481</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="H49" s="1"/>
@@ -5347,7 +5347,7 @@
         <v>1.5521514284737505E-19</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="H50" s="1"/>
@@ -5360,7 +5360,7 @@
         <v>5.0025205526249379E-21</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="H51" s="1"/>
@@ -5373,13 +5373,13 @@
         <v>3.2229590881760667E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="H53" s="1"/>
@@ -5396,17 +5396,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67644AD2-B82B-4CF0-B85E-F3756A511C5B}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="1" max="4" width="21.59765625" customWidth="1"/>
+    <col min="5" max="5" width="21.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>28</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>6.842105263157895E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>2.7027027027027029E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>3.0674846625766872E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>1.0638297872340425E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>5.499262864764933E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>1.128668171557562E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>1.2195121951219512E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Erste Verbesserungen von Hava. Vorwort wurde gemacht und neue Einleitung geschrieben.
</commit_message>
<xml_diff>
--- a/daten/datenVersuchSchön.xlsx
+++ b/daten/datenVersuchSchön.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelegli/Documents/git/maturaarbeit-Millikan/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE98497-953C-E141-9B5C-3425A2F96155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8558AAA-9E13-2940-B841-6D7AE5027677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{DABAE132-B07F-4807-8FB0-C17FFB8CB7E7}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Fehlerrechnung" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$Q$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Tröpfchen</t>
   </si>
@@ -76,9 +79,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>total</t>
   </si>
   <si>
     <t>q</t>
@@ -173,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -192,29 +192,110 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -312,7 +393,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$L$1</c:f>
+              <c:f>Tabelle1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -515,7 +596,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$2:$L$48</c:f>
+              <c:f>Tabelle1!$M$2:$M$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
@@ -1014,7 +1095,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$L$1</c:f>
+              <c:f>Tabelle1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1197,7 +1278,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$2:$L$48</c:f>
+              <c:f>Tabelle1!$M$2:$M$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
@@ -2732,16 +2813,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>503843</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>102979</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>127077</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>132612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1356276</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>51765</xdr:rowOff>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>268310</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>81398</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2768,16 +2849,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>862854</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>22411</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>151654</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>81678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>705971</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>56028</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>604371</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>115295</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3122,432 +3203,442 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{A1CAFB2B-394C-1A4D-83E0-AD25B6A37830}">
+  <we:reference id="a3b40b4f-8edf-490e-9df1-7e66f93912bf" version="1.1.0.0" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F711E3-911E-4A52-B155-A62E7AD9567F}">
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="N49" sqref="A1:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="20.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="9" customWidth="1"/>
+    <col min="2" max="14" width="20.6640625" style="12" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="11">
         <v>2.11954217888936E-5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="11">
         <v>2.0080321285139999E-4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="12">
         <v>23.59</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="12">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="12">
         <v>585</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="13">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="12">
         <v>886</v>
       </c>
-      <c r="K2">
-        <v>94364</v>
-      </c>
-      <c r="L2">
-        <v>3.2747980958213941E-19</v>
-      </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="K2" s="11">
         <f>F2/H2</f>
         <v>76973.68421052632</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="L2" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M2" s="12">
+        <v>3.2747980958213941E-19</v>
+      </c>
+      <c r="N2" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
         <v>2.158894645941278E-5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="11">
         <v>8.4602368866328257E-5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
         <v>23.16</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="12">
         <v>5.91</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <v>585</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="13">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <v>886</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="11">
+        <f>F3/H3</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="L3" s="12">
         <v>94364</v>
       </c>
-      <c r="L3">
+      <c r="M3" s="12">
         <v>1.5851685892692281E-19</v>
       </c>
-      <c r="M3">
+      <c r="N3" s="12">
         <v>1</v>
       </c>
-      <c r="N3" s="1">
-        <f t="shared" ref="N3:N48" si="0">F3/H3</f>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1.9833399444664819E-5</v>
+      </c>
+      <c r="C4" s="11">
+        <v>8.6805555555555559E-5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>25.21</v>
+      </c>
+      <c r="E4" s="12">
+        <v>5.76</v>
+      </c>
+      <c r="F4" s="12">
+        <v>585</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1.8099999999999999E-5</v>
+      </c>
+      <c r="H4" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I4" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J4" s="12">
+        <v>886</v>
+      </c>
+      <c r="K4" s="11">
+        <f>F4/H4</f>
         <v>76973.68421052632</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.9833399444664819E-5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8.6805555555555559E-5</v>
-      </c>
-      <c r="D4">
-        <v>25.21</v>
-      </c>
-      <c r="E4">
-        <v>5.76</v>
-      </c>
-      <c r="F4">
+      <c r="L4" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M4" s="12">
+        <v>1.5068138364557E-19</v>
+      </c>
+      <c r="N4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2.4715768660405332E-5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>9.3808630393996234E-5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>20.23</v>
+      </c>
+      <c r="E5" s="12">
+        <v>5.33</v>
+      </c>
+      <c r="F5" s="12">
         <v>585</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G5" s="13">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H5" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I5" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J4">
+      <c r="J5" s="12">
         <v>886</v>
       </c>
-      <c r="K4">
+      <c r="K5" s="11">
+        <f>F5/H5</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="L5" s="12">
         <v>94364</v>
       </c>
-      <c r="L4">
-        <v>1.5068138364557E-19</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <f t="shared" si="0"/>
-        <v>76973.68421052632</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.4715768660405332E-5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.3808630393996234E-5</v>
-      </c>
-      <c r="D5">
-        <v>20.23</v>
-      </c>
-      <c r="E5">
-        <v>5.33</v>
-      </c>
-      <c r="F5">
-        <v>585</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1.8099999999999999E-5</v>
-      </c>
-      <c r="H5" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I5" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J5">
-        <v>886</v>
-      </c>
-      <c r="K5">
-        <v>94364</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" si="0"/>
-        <v>76973.68421052632</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="11">
         <v>2.04164965291956E-5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="11">
         <f>0.0005/E6</f>
         <v>8.9126559714795006E-5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="12">
         <v>24.49</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="12">
         <v>5.61</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>585</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="13">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="12">
         <v>886</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="11">
+        <f>F6/H6</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="L6" s="12">
         <v>94364</v>
       </c>
-      <c r="L6">
+      <c r="M6" s="12">
         <v>1.5772476256952349E-19</v>
       </c>
-      <c r="M6">
+      <c r="N6" s="12">
         <v>1</v>
       </c>
-      <c r="N6" s="1">
-        <f t="shared" si="0"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1.975503753457132E-5</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1.9685039370070001E-4</v>
+      </c>
+      <c r="D7" s="12">
+        <v>25.31</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2.54</v>
+      </c>
+      <c r="F7" s="12">
+        <v>585</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1.8099999999999999E-5</v>
+      </c>
+      <c r="H7" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I7" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J7" s="12">
+        <v>886</v>
+      </c>
+      <c r="K7" s="11">
+        <f>F7/H7</f>
         <v>76973.68421052632</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.975503753457132E-5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.9685039370070001E-4</v>
-      </c>
-      <c r="D7">
-        <v>25.31</v>
-      </c>
-      <c r="E7">
-        <v>2.54</v>
-      </c>
-      <c r="F7">
+      <c r="L7" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M7" s="12">
+        <v>3.052773302419662E-19</v>
+      </c>
+      <c r="N7" s="12">
+        <v>2</v>
+      </c>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2.044153720359771E-5</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1.97628458498E-4</v>
+      </c>
+      <c r="D8" s="12">
+        <v>24.46</v>
+      </c>
+      <c r="E8" s="12">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F8" s="12">
         <v>585</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G8" s="13">
         <v>1.8099999999999999E-5</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H8" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I8" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J7">
+      <c r="J8" s="12">
         <v>886</v>
       </c>
-      <c r="K7">
+      <c r="K8" s="11">
+        <f>F8/H8</f>
+        <v>76973.68421052632</v>
+      </c>
+      <c r="L8" s="12">
         <v>94364</v>
       </c>
-      <c r="L7">
-        <v>3.052773302419662E-19</v>
-      </c>
-      <c r="M7">
+      <c r="M8" s="12">
+        <v>3.1423605559845701E-19</v>
+      </c>
+      <c r="N8" s="12">
         <v>2</v>
       </c>
-      <c r="N7" s="1">
-        <f t="shared" si="0"/>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1.8429782528566169E-5</v>
+      </c>
+      <c r="C9" s="11">
+        <v>9.328358208955224E-5</v>
+      </c>
+      <c r="D9" s="12">
+        <v>27.13</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5.36</v>
+      </c>
+      <c r="F9" s="12">
+        <v>585</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1.8099999999999999E-5</v>
+      </c>
+      <c r="H9" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I9" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J9" s="12">
+        <v>886</v>
+      </c>
+      <c r="K9" s="11">
+        <f>F9/H9</f>
         <v>76973.68421052632</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2.044153720359771E-5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.97628458498E-4</v>
-      </c>
-      <c r="D8">
-        <v>24.46</v>
-      </c>
-      <c r="E8">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="F8">
-        <v>585</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1.8099999999999999E-5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J8">
-        <v>886</v>
-      </c>
-      <c r="K8">
+      <c r="L9" s="12">
         <v>94364</v>
       </c>
-      <c r="L8">
-        <v>3.1423605559845701E-19</v>
-      </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>76973.68421052632</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.8429782528566169E-5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.328358208955224E-5</v>
-      </c>
-      <c r="D9">
-        <v>27.13</v>
-      </c>
-      <c r="E9">
-        <v>5.36</v>
-      </c>
-      <c r="F9">
-        <v>585</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1.8099999999999999E-5</v>
-      </c>
-      <c r="H9" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I9" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J9">
-        <v>886</v>
-      </c>
-      <c r="K9">
-        <v>94364</v>
-      </c>
-      <c r="L9">
+      <c r="M9" s="12">
         <v>1.5046225734477661E-19</v>
       </c>
-      <c r="M9">
+      <c r="N9" s="12">
         <v>1</v>
       </c>
-      <c r="N9" s="1">
-        <f t="shared" si="0"/>
-        <v>76973.68421052632</v>
-      </c>
-      <c r="O9"/>
+      <c r="O9" s="7"/>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
@@ -3560,310 +3651,317 @@
       <c r="Y9"/>
       <c r="Z9"/>
       <c r="AA9"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="AB9"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="11">
         <v>1.708817498291182E-5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="11">
         <v>1.2562814070350001E-4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
         <v>29.26</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="12">
         <v>3.98</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <v>586</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="13">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="12">
         <v>886</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="11">
+        <f>F10/H10</f>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="L10" s="12">
         <v>94364</v>
       </c>
-      <c r="L10">
+      <c r="M10" s="12">
         <v>1.8492070982804951E-19</v>
       </c>
-      <c r="M10">
+      <c r="N10" s="12">
         <v>1</v>
       </c>
-      <c r="N10" s="1">
-        <f t="shared" si="0"/>
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1.692620176032498E-5</v>
+      </c>
+      <c r="C11" s="11">
+        <v>3.9062500000000002E-4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>29.54</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1.28</v>
+      </c>
+      <c r="F11" s="12">
+        <v>586</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1.8240000000000002E-5</v>
+      </c>
+      <c r="H11" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I11" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J11" s="12">
+        <v>886</v>
+      </c>
+      <c r="K11" s="11">
+        <f>F11/H11</f>
         <v>77105.263157894733</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.692620176032498E-5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.9062500000000002E-4</v>
-      </c>
-      <c r="D11">
-        <v>29.54</v>
-      </c>
-      <c r="E11">
-        <v>1.28</v>
-      </c>
-      <c r="F11">
+      <c r="L11" s="12">
+        <v>94364</v>
+      </c>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1.2333497779970399E-5</v>
+      </c>
+      <c r="C12" s="11">
+        <v>1.121076233183E-4</v>
+      </c>
+      <c r="D12" s="12">
+        <v>40.54</v>
+      </c>
+      <c r="E12" s="12">
+        <v>4.46</v>
+      </c>
+      <c r="F12" s="12">
         <v>586</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="13">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I12" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J11">
+      <c r="J12" s="12">
         <v>886</v>
       </c>
-      <c r="K11">
+      <c r="K12" s="11">
+        <f>F12/H12</f>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="L12" s="12">
         <v>94364</v>
       </c>
-      <c r="N11" s="1">
-        <f t="shared" si="0"/>
+      <c r="M12" s="12">
+        <v>1.2938659935743371E-19</v>
+      </c>
+      <c r="N12" s="12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1.289324394017535E-5</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1.295336787564E-4</v>
+      </c>
+      <c r="D13" s="12">
+        <v>38.78</v>
+      </c>
+      <c r="E13" s="12">
+        <v>3.86</v>
+      </c>
+      <c r="F13" s="12">
+        <v>586</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1.8240000000000002E-5</v>
+      </c>
+      <c r="H13" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I13" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J13" s="12">
+        <v>886</v>
+      </c>
+      <c r="K13" s="11">
+        <f>F13/H13</f>
         <v>77105.263157894733</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1.2333497779970399E-5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.121076233183E-4</v>
-      </c>
-      <c r="D12">
-        <v>40.54</v>
-      </c>
-      <c r="E12">
-        <v>4.46</v>
-      </c>
-      <c r="F12">
+      <c r="L13" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M13" s="12">
+        <v>1.5267483032452281E-19</v>
+      </c>
+      <c r="N13" s="12">
+        <v>1</v>
+      </c>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1.316135825217162E-5</v>
+      </c>
+      <c r="C14" s="11">
+        <v>2.2624434389139999E-4</v>
+      </c>
+      <c r="D14" s="12">
+        <v>37.99</v>
+      </c>
+      <c r="E14" s="12">
+        <v>2.21</v>
+      </c>
+      <c r="F14" s="12">
         <v>586</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G14" s="13">
         <v>1.8240000000000002E-5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H14" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I14" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J12">
+      <c r="J14" s="12">
         <v>886</v>
       </c>
-      <c r="K12">
+      <c r="K14" s="11">
+        <f>F14/H14</f>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="L14" s="12">
         <v>94364</v>
       </c>
-      <c r="L12">
-        <v>1.2938659935743371E-19</v>
-      </c>
-      <c r="M12">
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1.151012891344383E-5</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1.262626262626E-4</v>
+      </c>
+      <c r="D15" s="12">
+        <v>43.44</v>
+      </c>
+      <c r="E15" s="12">
+        <v>3.96</v>
+      </c>
+      <c r="F15" s="12">
+        <v>586</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1.8240000000000002E-5</v>
+      </c>
+      <c r="H15" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I15" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J15" s="12">
+        <v>886</v>
+      </c>
+      <c r="K15" s="11">
+        <f>F15/H15</f>
+        <v>77105.263157894733</v>
+      </c>
+      <c r="L15" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M15" s="12">
+        <v>1.365537769282638E-19</v>
+      </c>
+      <c r="N15" s="12">
         <v>1</v>
       </c>
-      <c r="N12" s="1">
-        <f t="shared" si="0"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1.575299306868305E-5</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1.210653753026E-4</v>
+      </c>
+      <c r="D16" s="12">
+        <v>31.74</v>
+      </c>
+      <c r="E16" s="12">
+        <v>4.13</v>
+      </c>
+      <c r="F16" s="12">
+        <v>586</v>
+      </c>
+      <c r="G16" s="13">
+        <v>1.8240000000000002E-5</v>
+      </c>
+      <c r="H16" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I16" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J16" s="12">
+        <v>886</v>
+      </c>
+      <c r="K16" s="11">
+        <f>F16/H16</f>
         <v>77105.263157894733</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.289324394017535E-5</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.295336787564E-4</v>
-      </c>
-      <c r="D13">
-        <v>38.78</v>
-      </c>
-      <c r="E13">
-        <v>3.86</v>
-      </c>
-      <c r="F13">
-        <v>586</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1.8240000000000002E-5</v>
-      </c>
-      <c r="H13" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I13" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J13">
-        <v>886</v>
-      </c>
-      <c r="K13">
+      <c r="L16" s="12">
         <v>94364</v>
       </c>
-      <c r="L13">
-        <v>1.5267483032452281E-19</v>
-      </c>
-      <c r="M13">
+      <c r="M16" s="12">
+        <v>1.679480167697637E-19</v>
+      </c>
+      <c r="N16" s="12">
         <v>1</v>
       </c>
-      <c r="N13" s="1">
-        <f t="shared" si="0"/>
-        <v>77105.263157894733</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.316135825217162E-5</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2.2624434389139999E-4</v>
-      </c>
-      <c r="D14">
-        <v>37.99</v>
-      </c>
-      <c r="E14">
-        <v>2.21</v>
-      </c>
-      <c r="F14">
-        <v>586</v>
-      </c>
-      <c r="G14" s="6">
-        <v>1.8240000000000002E-5</v>
-      </c>
-      <c r="H14" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I14" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J14">
-        <v>886</v>
-      </c>
-      <c r="K14">
-        <v>94364</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="0"/>
-        <v>77105.263157894733</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.151012891344383E-5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1.262626262626E-4</v>
-      </c>
-      <c r="D15">
-        <v>43.44</v>
-      </c>
-      <c r="E15">
-        <v>3.96</v>
-      </c>
-      <c r="F15">
-        <v>586</v>
-      </c>
-      <c r="G15" s="6">
-        <v>1.8240000000000002E-5</v>
-      </c>
-      <c r="H15" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I15" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J15">
-        <v>886</v>
-      </c>
-      <c r="K15">
-        <v>94364</v>
-      </c>
-      <c r="L15">
-        <v>1.365537769282638E-19</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="0"/>
-        <v>77105.263157894733</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.575299306868305E-5</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.210653753026E-4</v>
-      </c>
-      <c r="D16">
-        <v>31.74</v>
-      </c>
-      <c r="E16">
-        <v>4.13</v>
-      </c>
-      <c r="F16">
-        <v>586</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1.8240000000000002E-5</v>
-      </c>
-      <c r="H16" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I16" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J16">
-        <v>886</v>
-      </c>
-      <c r="K16">
-        <v>94364</v>
-      </c>
-      <c r="L16">
-        <v>1.679480167697637E-19</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="0"/>
-        <v>77105.263157894733</v>
-      </c>
-      <c r="O16"/>
+      <c r="O16" s="7"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
@@ -3876,222 +3974,227 @@
       <c r="Y16"/>
       <c r="Z16"/>
       <c r="AA16"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="AB16"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="11">
         <v>1.8109380659181451E-5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="11">
         <v>2.2624434389139999E-4</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="12">
         <v>27.61</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="12">
         <v>2.21</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="12">
         <v>580</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="13">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="12">
         <v>886</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="11">
+        <f>F17/H17</f>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="L17" s="12">
         <v>94364</v>
       </c>
-      <c r="L17">
+      <c r="M17" s="12">
         <v>3.3115626946853271E-19</v>
       </c>
-      <c r="M17">
+      <c r="N17" s="12">
         <v>2</v>
       </c>
-      <c r="N17" s="1">
-        <f t="shared" si="0"/>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1.212709192335678E-5</v>
+      </c>
+      <c r="C18" s="11">
+        <v>4.5045045045039999E-4</v>
+      </c>
+      <c r="D18" s="12">
+        <v>41.23</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F18" s="12">
+        <v>580</v>
+      </c>
+      <c r="G18" s="13">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H18" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I18" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J18" s="12">
+        <v>886</v>
+      </c>
+      <c r="K18" s="11">
+        <f>F18/H18</f>
         <v>76315.789473684214</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.212709192335678E-5</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="L18" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M18" s="12">
+        <v>4.7852879920201003E-19</v>
+      </c>
+      <c r="N18" s="12">
+        <v>3</v>
+      </c>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1.07781849536538E-5</v>
+      </c>
+      <c r="C19" s="11">
         <v>4.5045045045039999E-4</v>
       </c>
-      <c r="D18">
-        <v>41.23</v>
-      </c>
-      <c r="E18">
+      <c r="D19" s="12">
+        <v>46.39</v>
+      </c>
+      <c r="E19" s="12">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F18">
+      <c r="F19" s="12">
         <v>580</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G19" s="13">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H19" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I19" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J18">
+      <c r="J19" s="12">
         <v>886</v>
       </c>
-      <c r="K18">
+      <c r="K19" s="11">
+        <f>F19/H19</f>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="L19" s="12">
         <v>94364</v>
       </c>
-      <c r="L18">
-        <v>4.7852879920201003E-19</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="0"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11">
+        <v>1.065189603749468E-5</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2.8409090909090002E-4</v>
+      </c>
+      <c r="D20" s="12">
+        <v>46.94</v>
+      </c>
+      <c r="E20" s="12">
+        <v>1.76</v>
+      </c>
+      <c r="F20" s="12">
+        <v>580</v>
+      </c>
+      <c r="G20" s="13">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H20" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I20" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J20" s="12">
+        <v>886</v>
+      </c>
+      <c r="K20" s="11">
+        <f>F20/H20</f>
         <v>76315.789473684214</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.07781849536538E-5</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4.5045045045039999E-4</v>
-      </c>
-      <c r="D19">
-        <v>46.39</v>
-      </c>
-      <c r="E19">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="F19">
+      <c r="L20" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M20" s="12">
+        <v>2.7853483615976351E-19</v>
+      </c>
+      <c r="N20" s="12">
+        <v>2</v>
+      </c>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1.147842056932966E-5</v>
+      </c>
+      <c r="C21" s="11">
+        <v>5.6179775280890002E-4</v>
+      </c>
+      <c r="D21" s="12">
+        <v>43.56</v>
+      </c>
+      <c r="E21" s="12">
+        <v>0.89</v>
+      </c>
+      <c r="F21" s="12">
         <v>580</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G21" s="13">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H21" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I21" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J19">
+      <c r="J21" s="12">
         <v>886</v>
       </c>
-      <c r="K19">
+      <c r="K21" s="11">
+        <f>F21/H21</f>
+        <v>76315.789473684214</v>
+      </c>
+      <c r="L21" s="12">
         <v>94364</v>
       </c>
-      <c r="N19" s="1">
-        <f t="shared" si="0"/>
-        <v>76315.789473684214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.065189603749468E-5</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2.8409090909090002E-4</v>
-      </c>
-      <c r="D20">
-        <v>46.94</v>
-      </c>
-      <c r="E20">
-        <v>1.76</v>
-      </c>
-      <c r="F20">
-        <v>580</v>
-      </c>
-      <c r="G20" s="6">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H20" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I20" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J20">
-        <v>886</v>
-      </c>
-      <c r="K20">
-        <v>94364</v>
-      </c>
-      <c r="L20">
-        <v>2.7853483615976351E-19</v>
-      </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="0"/>
-        <v>76315.789473684214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.147842056932966E-5</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5.6179775280890002E-4</v>
-      </c>
-      <c r="D21">
-        <v>43.56</v>
-      </c>
-      <c r="E21">
-        <v>0.89</v>
-      </c>
-      <c r="F21">
-        <v>580</v>
-      </c>
-      <c r="G21" s="6">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H21" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I21" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J21">
-        <v>886</v>
-      </c>
-      <c r="K21">
-        <v>94364</v>
-      </c>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21" s="1">
-        <f t="shared" si="0"/>
-        <v>76315.789473684214</v>
-      </c>
-      <c r="O21"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="7"/>
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
@@ -4104,1286 +4207,1300 @@
       <c r="Y21"/>
       <c r="Z21"/>
       <c r="AA21"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="AB21"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="11">
         <v>1.11656989727557E-5</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="11">
         <v>1.179245283018E-4</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="12">
         <v>44.78</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="12">
         <v>4.24</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="12">
         <v>583</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="13">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="12">
         <v>886</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="11">
+        <f>F22/H22</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L22" s="12">
         <v>94364</v>
       </c>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11">
+        <v>1.4033118158854901E-5</v>
+      </c>
+      <c r="C23" s="11">
+        <v>2.427184466019E-4</v>
+      </c>
+      <c r="D23" s="12">
+        <v>35.630000000000003</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2.06</v>
+      </c>
+      <c r="F23" s="12">
+        <v>583</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1.8219999999999998E-5</v>
+      </c>
+      <c r="H23" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I23" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J23" s="12">
+        <v>886</v>
+      </c>
+      <c r="K23" s="11">
+        <f>F23/H23</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.4033118158854901E-5</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2.427184466019E-4</v>
-      </c>
-      <c r="D23">
-        <v>35.630000000000003</v>
-      </c>
-      <c r="E23">
-        <v>2.06</v>
-      </c>
-      <c r="F23">
+      <c r="L23" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M23" s="12">
+        <v>2.9254518781664188E-19</v>
+      </c>
+      <c r="N23" s="12">
+        <v>2</v>
+      </c>
+      <c r="O23" s="7"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11">
+        <v>1.282380097460887E-5</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1.2562814070350001E-4</v>
+      </c>
+      <c r="D24" s="12">
+        <v>38.99</v>
+      </c>
+      <c r="E24" s="12">
+        <v>3.98</v>
+      </c>
+      <c r="F24" s="12">
         <v>583</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G24" s="13">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H24" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I24" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J23">
+      <c r="J24" s="12">
         <v>886</v>
       </c>
-      <c r="K23">
+      <c r="K24" s="11">
+        <f>F24/H24</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L24" s="12">
         <v>94364</v>
       </c>
-      <c r="L23">
-        <v>2.9254518781664188E-19</v>
-      </c>
-      <c r="M23">
+      <c r="M24" s="12">
+        <v>1.483515883555309E-19</v>
+      </c>
+      <c r="N24" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11">
+        <v>1.304461257500652E-5</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3.9682539682530001E-4</v>
+      </c>
+      <c r="D25" s="12">
+        <v>38.33</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.26</v>
+      </c>
+      <c r="F25" s="12">
+        <v>583</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1.8219999999999998E-5</v>
+      </c>
+      <c r="H25" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I25" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J25" s="12">
+        <v>886</v>
+      </c>
+      <c r="K25" s="11">
+        <f>F25/H25</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L25" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M25" s="12">
+        <v>4.4434402544902837E-19</v>
+      </c>
+      <c r="N25" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11">
+        <v>1.446759259259259E-5</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2.4875621890539998E-4</v>
+      </c>
+      <c r="D26" s="12">
+        <v>34.56</v>
+      </c>
+      <c r="E26" s="12">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F26" s="12">
+        <v>583</v>
+      </c>
+      <c r="G26" s="13">
+        <v>1.8219999999999998E-5</v>
+      </c>
+      <c r="H26" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I26" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J26" s="12">
+        <v>886</v>
+      </c>
+      <c r="K26" s="11">
+        <f>F26/H26</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L26" s="12">
+        <v>94364</v>
+      </c>
+      <c r="M26" s="12">
+        <v>3.0617078747401381E-19</v>
+      </c>
+      <c r="N26" s="12">
         <v>2</v>
       </c>
-      <c r="N23" s="1">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1.032204789430223E-5</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2.3923444976069999E-4</v>
+      </c>
+      <c r="D27" s="12">
+        <v>48.44</v>
+      </c>
+      <c r="E27" s="12">
+        <v>2.09</v>
+      </c>
+      <c r="F27" s="12">
+        <v>583</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1.8219999999999998E-5</v>
+      </c>
+      <c r="H27" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I27" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J27" s="12">
+        <v>886</v>
+      </c>
+      <c r="K27" s="11">
+        <f>F27/H27</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.282380097460887E-5</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.2562814070350001E-4</v>
-      </c>
-      <c r="D24">
-        <v>38.99</v>
-      </c>
-      <c r="E24">
-        <v>3.98</v>
-      </c>
-      <c r="F24">
+      <c r="L27" s="12">
+        <v>94364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11">
+        <v>1.047339757017176E-5</v>
+      </c>
+      <c r="C28" s="11">
+        <v>2.6178010471200001E-4</v>
+      </c>
+      <c r="D28" s="12">
+        <v>47.74</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1.91</v>
+      </c>
+      <c r="F28" s="12">
         <v>583</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G28" s="13">
         <v>1.8219999999999998E-5</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H28" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I28" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J24">
+      <c r="J28" s="12">
         <v>886</v>
       </c>
-      <c r="K24">
+      <c r="K28" s="11">
+        <f>F28/H28</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L28" s="12">
         <v>94364</v>
       </c>
-      <c r="L24">
-        <v>1.483515883555309E-19</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.304461257500652E-5</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3.9682539682530001E-4</v>
-      </c>
-      <c r="D25">
-        <v>38.33</v>
-      </c>
-      <c r="E25">
-        <v>1.26</v>
-      </c>
-      <c r="F25">
-        <v>583</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1.8219999999999998E-5</v>
-      </c>
-      <c r="H25" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I25" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J25">
-        <v>886</v>
-      </c>
-      <c r="K25">
-        <v>94364</v>
-      </c>
-      <c r="L25">
-        <v>4.4434402544902837E-19</v>
-      </c>
-      <c r="M25">
-        <v>3</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.446759259259259E-5</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.4875621890539998E-4</v>
-      </c>
-      <c r="D26">
-        <v>34.56</v>
-      </c>
-      <c r="E26">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="F26">
-        <v>583</v>
-      </c>
-      <c r="G26" s="6">
-        <v>1.8219999999999998E-5</v>
-      </c>
-      <c r="H26" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I26" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J26">
-        <v>886</v>
-      </c>
-      <c r="K26">
-        <v>94364</v>
-      </c>
-      <c r="L26">
-        <v>3.0617078747401381E-19</v>
-      </c>
-      <c r="M26">
-        <v>2</v>
-      </c>
-      <c r="N26" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.032204789430223E-5</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2.3923444976069999E-4</v>
-      </c>
-      <c r="D27">
-        <v>48.44</v>
-      </c>
-      <c r="E27">
-        <v>2.09</v>
-      </c>
-      <c r="F27">
-        <v>583</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1.8219999999999998E-5</v>
-      </c>
-      <c r="H27" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I27" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J27">
-        <v>886</v>
-      </c>
-      <c r="K27">
-        <v>94364</v>
-      </c>
-      <c r="N27" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1.047339757017176E-5</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2.6178010471200001E-4</v>
-      </c>
-      <c r="D28">
-        <v>47.74</v>
-      </c>
-      <c r="E28">
-        <v>1.91</v>
-      </c>
-      <c r="F28">
-        <v>583</v>
-      </c>
-      <c r="G28" s="6">
-        <v>1.8219999999999998E-5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I28" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J28">
-        <v>886</v>
-      </c>
-      <c r="K28">
-        <v>94364</v>
-      </c>
-      <c r="N28" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29">
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="11">
         <f>0.0005/D29</f>
         <v>3.6284470246734402E-5</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="11">
         <f>0.0005/E29</f>
         <v>3.048780487804878E-4</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="12">
         <v>13.78</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="12">
         <v>1.64</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="12">
         <v>583</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="13">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="12">
         <v>886</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="11">
+        <f>F29/H29</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L29" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="N29" s="1">
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" ref="B30:B40" si="0">0.0005/D30</f>
+        <v>3.3579583613163193E-5</v>
+      </c>
+      <c r="C30" s="11">
+        <f t="shared" ref="C30:C40" si="1">0.0005/E30</f>
+        <v>3.95882818685669E-5</v>
+      </c>
+      <c r="D30" s="12">
+        <v>14.89</v>
+      </c>
+      <c r="E30" s="12">
+        <v>12.63</v>
+      </c>
+      <c r="F30" s="12">
+        <v>583</v>
+      </c>
+      <c r="G30" s="13">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H30" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I30" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J30" s="12">
+        <v>886</v>
+      </c>
+      <c r="K30" s="11">
+        <f>F30/H30</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L30" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M30" s="12">
+        <v>1.4554623175668291E-19</v>
+      </c>
+      <c r="N30" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="11">
         <f t="shared" si="0"/>
+        <v>1.4744913005013272E-5</v>
+      </c>
+      <c r="C31" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0438413361169103E-4</v>
+      </c>
+      <c r="D31" s="12">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="E31" s="12">
+        <v>4.79</v>
+      </c>
+      <c r="F31" s="12">
+        <v>583</v>
+      </c>
+      <c r="G31" s="13">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H31" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I31" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J31" s="12">
+        <v>886</v>
+      </c>
+      <c r="K31" s="11">
+        <f>F31/H31</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <f t="shared" ref="B30:B40" si="1">0.0005/D30</f>
-        <v>3.3579583613163193E-5</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" ref="C30:C40" si="2">0.0005/E30</f>
-        <v>3.95882818685669E-5</v>
-      </c>
-      <c r="D30">
-        <v>14.89</v>
-      </c>
-      <c r="E30">
-        <v>12.63</v>
-      </c>
-      <c r="F30">
+      <c r="L31" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M31" s="12">
+        <v>1.3963446372113281E-19</v>
+      </c>
+      <c r="N31" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="11">
+        <f t="shared" si="0"/>
+        <v>2.8851702250432778E-5</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="shared" si="1"/>
+        <v>5.2192066805845514E-5</v>
+      </c>
+      <c r="D32" s="12">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="E32" s="12">
+        <v>9.58</v>
+      </c>
+      <c r="F32" s="12">
         <v>583</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G32" s="13">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H32" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I32" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J30">
+      <c r="J32" s="12">
         <v>886</v>
       </c>
-      <c r="K30">
+      <c r="K32" s="11">
+        <f>F32/H32</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L32" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L30">
-        <v>1.4554623175668291E-19</v>
-      </c>
-      <c r="M30">
+      <c r="M32" s="12">
+        <v>1.4673753039611549E-19</v>
+      </c>
+      <c r="N32" s="12">
         <v>1</v>
       </c>
-      <c r="N30" s="1">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11">
         <f t="shared" si="0"/>
+        <v>3.0618493570116355E-5</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" si="1"/>
+        <v>5.3995680345572353E-5</v>
+      </c>
+      <c r="D33" s="12">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="E33" s="12">
+        <v>9.26</v>
+      </c>
+      <c r="F33" s="12">
+        <v>583</v>
+      </c>
+      <c r="G33" s="13">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H33" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I33" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J33" s="12">
+        <v>886</v>
+      </c>
+      <c r="K33" s="11">
+        <f>F33/H33</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="L33" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M33" s="12">
+        <v>1.5897872941404839E-19</v>
+      </c>
+      <c r="N33" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11">
+        <f t="shared" si="0"/>
+        <v>2.6695141484249868E-5</v>
+      </c>
+      <c r="C34" s="11">
         <f t="shared" si="1"/>
-        <v>1.4744913005013272E-5</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0438413361169103E-4</v>
-      </c>
-      <c r="D31">
-        <v>33.909999999999997</v>
-      </c>
-      <c r="E31">
-        <v>4.79</v>
-      </c>
-      <c r="F31">
+        <v>5.8207217694994179E-5</v>
+      </c>
+      <c r="D34" s="12">
+        <v>18.73</v>
+      </c>
+      <c r="E34" s="12">
+        <v>8.59</v>
+      </c>
+      <c r="F34" s="12">
         <v>583</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G34" s="13">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H34" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I34" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J31">
+      <c r="J34" s="12">
         <v>886</v>
       </c>
-      <c r="K31">
+      <c r="K34" s="11">
+        <f>F34/H34</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L34" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L31">
-        <v>1.3963446372113281E-19</v>
-      </c>
-      <c r="M31">
+      <c r="M34" s="12">
+        <v>1.4641553540058561E-19</v>
+      </c>
+      <c r="N34" s="12">
         <v>1</v>
       </c>
-      <c r="N31" s="1">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11">
         <f t="shared" si="0"/>
+        <v>2.9779630732578919E-5</v>
+      </c>
+      <c r="C35" s="11">
+        <f t="shared" si="1"/>
+        <v>5.3418803418803426E-5</v>
+      </c>
+      <c r="D35" s="12">
+        <v>16.79</v>
+      </c>
+      <c r="E35" s="12">
+        <v>9.36</v>
+      </c>
+      <c r="F35" s="12">
+        <v>583</v>
+      </c>
+      <c r="G35" s="13">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H35" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I35" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J35" s="12">
+        <v>886</v>
+      </c>
+      <c r="K35" s="11">
+        <f>F35/H35</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
+      <c r="L35" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M35" s="12">
+        <v>1.536419009789623E-19</v>
+      </c>
+      <c r="N35" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="11">
+        <f t="shared" si="0"/>
+        <v>2.7917364600781685E-5</v>
+      </c>
+      <c r="C36" s="11">
         <f t="shared" si="1"/>
-        <v>2.8851702250432778E-5</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="2"/>
-        <v>5.2192066805845514E-5</v>
-      </c>
-      <c r="D32">
-        <v>17.329999999999998</v>
-      </c>
-      <c r="E32">
-        <v>9.58</v>
-      </c>
-      <c r="F32">
+        <v>5.76036866359447E-5</v>
+      </c>
+      <c r="D36" s="12">
+        <v>17.91</v>
+      </c>
+      <c r="E36" s="12">
+        <v>8.68</v>
+      </c>
+      <c r="F36" s="12">
         <v>583</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G36" s="13">
         <v>1.8159999999999999E-5</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H36" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I36" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J32">
+      <c r="J36" s="12">
         <v>886</v>
       </c>
-      <c r="K32">
+      <c r="K36" s="11">
+        <f>F36/H36</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L36" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L32">
-        <v>1.4673753039611549E-19</v>
-      </c>
-      <c r="M32">
+      <c r="M36" s="12">
+        <v>1.5168780241725071E-19</v>
+      </c>
+      <c r="N36" s="12">
         <v>1</v>
       </c>
-      <c r="N32" s="1">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11">
         <f t="shared" si="0"/>
+        <v>3.0138637733574443E-5</v>
+      </c>
+      <c r="C37" s="11">
+        <f t="shared" si="1"/>
+        <v>5.8072009291521493E-5</v>
+      </c>
+      <c r="D37" s="12">
+        <v>16.59</v>
+      </c>
+      <c r="E37" s="12">
+        <v>8.61</v>
+      </c>
+      <c r="F37" s="12">
+        <v>583</v>
+      </c>
+      <c r="G37" s="13">
+        <v>1.8159999999999999E-5</v>
+      </c>
+      <c r="H37" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I37" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J37" s="12">
+        <v>886</v>
+      </c>
+      <c r="K37" s="11">
+        <f>F37/H37</f>
         <v>76710.526315789481</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
+      <c r="L37" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M37" s="12">
+        <v>1.641171292859742E-19</v>
+      </c>
+      <c r="N37" s="12">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>37</v>
+      </c>
+      <c r="B38" s="11">
+        <f t="shared" si="0"/>
+        <v>1.8946570670708603E-5</v>
+      </c>
+      <c r="C38" s="11">
         <f t="shared" si="1"/>
-        <v>3.0618493570116355E-5</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="2"/>
-        <v>5.3995680345572353E-5</v>
-      </c>
-      <c r="D33">
-        <v>16.329999999999998</v>
-      </c>
-      <c r="E33">
-        <v>9.26</v>
-      </c>
-      <c r="F33">
-        <v>583</v>
-      </c>
-      <c r="G33" s="6">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H33" s="1">
+        <v>5.3191489361702129E-4</v>
+      </c>
+      <c r="D38" s="12">
+        <v>26.39</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="F38" s="12">
+        <v>582</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H38" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I38" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J33">
+      <c r="J38" s="12">
         <v>886</v>
       </c>
-      <c r="K33">
+      <c r="K38" s="11">
+        <f>F38/H38</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L38" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L33">
-        <v>1.5897872941404839E-19</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33" s="1">
+      <c r="M38" s="12">
+        <v>7.6660747025858679E-19</v>
+      </c>
+      <c r="N38" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11">
         <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
+        <v>1.8982536066818528E-5</v>
+      </c>
+      <c r="C39" s="11">
         <f t="shared" si="1"/>
-        <v>2.6695141484249868E-5</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" si="2"/>
-        <v>5.8207217694994179E-5</v>
-      </c>
-      <c r="D34">
-        <v>18.73</v>
-      </c>
-      <c r="E34">
-        <v>8.59</v>
-      </c>
-      <c r="F34">
-        <v>583</v>
-      </c>
-      <c r="G34" s="6">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H34" s="1">
+        <v>3.5460992907801421E-4</v>
+      </c>
+      <c r="D39" s="12">
+        <v>26.34</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1.41</v>
+      </c>
+      <c r="F39" s="12">
+        <v>582</v>
+      </c>
+      <c r="G39" s="11">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H39" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I39" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J34">
+      <c r="J39" s="12">
         <v>886</v>
       </c>
-      <c r="K34">
+      <c r="K39" s="11">
+        <f>F39/H39</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L39" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L34">
-        <v>1.4641553540058561E-19</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34" s="1">
+      <c r="M39" s="12">
+        <v>5.2055514577343985E-19</v>
+      </c>
+      <c r="N39" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="11">
         <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
+        <v>1.6539861065167053E-5</v>
+      </c>
+      <c r="C40" s="11">
         <f t="shared" si="1"/>
-        <v>2.9779630732578919E-5</v>
-      </c>
-      <c r="C35" s="1">
-        <f t="shared" si="2"/>
-        <v>5.3418803418803426E-5</v>
-      </c>
-      <c r="D35">
-        <v>16.79</v>
-      </c>
-      <c r="E35">
-        <v>9.36</v>
-      </c>
-      <c r="F35">
-        <v>583</v>
-      </c>
-      <c r="G35" s="6">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H35" s="1">
+        <v>3.3112582781456954E-4</v>
+      </c>
+      <c r="D40" s="12">
+        <v>30.23</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1.51</v>
+      </c>
+      <c r="F40" s="12">
+        <v>582</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H40" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I40" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J35">
+      <c r="J40" s="12">
         <v>886</v>
       </c>
-      <c r="K35">
+      <c r="K40" s="11">
+        <f>F40/H40</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L40" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L35">
-        <v>1.536419009789623E-19</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1">
-        <f t="shared" si="1"/>
-        <v>2.7917364600781685E-5</v>
-      </c>
-      <c r="C36" s="1">
-        <f t="shared" si="2"/>
-        <v>5.76036866359447E-5</v>
-      </c>
-      <c r="D36">
-        <v>17.91</v>
-      </c>
-      <c r="E36">
-        <v>8.68</v>
-      </c>
-      <c r="F36">
-        <v>583</v>
-      </c>
-      <c r="G36" s="6">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H36" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I36" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J36">
-        <v>886</v>
-      </c>
-      <c r="K36">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L36">
-        <v>1.5168780241725071E-19</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1">
-        <f t="shared" si="1"/>
-        <v>3.0138637733574443E-5</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="2"/>
-        <v>5.8072009291521493E-5</v>
-      </c>
-      <c r="D37">
-        <v>16.59</v>
-      </c>
-      <c r="E37">
-        <v>8.61</v>
-      </c>
-      <c r="F37">
-        <v>583</v>
-      </c>
-      <c r="G37" s="6">
-        <v>1.8159999999999999E-5</v>
-      </c>
-      <c r="H37" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I37" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J37">
-        <v>886</v>
-      </c>
-      <c r="K37">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L37">
-        <v>1.641171292859742E-19</v>
-      </c>
-      <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="N37" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8946570670708603E-5</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="2"/>
-        <v>5.3191489361702129E-4</v>
-      </c>
-      <c r="D38">
-        <v>26.39</v>
-      </c>
-      <c r="E38">
-        <v>0.94</v>
-      </c>
-      <c r="F38">
-        <v>582</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H38" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I38" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J38">
-        <v>886</v>
-      </c>
-      <c r="K38">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L38">
-        <v>7.6660747025858679E-19</v>
-      </c>
-      <c r="M38">
-        <v>5</v>
-      </c>
-      <c r="N38" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8982536066818528E-5</v>
-      </c>
-      <c r="C39" s="1">
-        <f t="shared" si="2"/>
-        <v>3.5460992907801421E-4</v>
-      </c>
-      <c r="D39">
-        <v>26.34</v>
-      </c>
-      <c r="E39">
-        <v>1.41</v>
-      </c>
-      <c r="F39">
-        <v>582</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H39" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I39" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J39">
-        <v>886</v>
-      </c>
-      <c r="K39">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L39">
-        <v>5.2055514577343985E-19</v>
-      </c>
-      <c r="M39">
+      <c r="M40" s="12">
+        <v>4.4242549593716838E-19</v>
+      </c>
+      <c r="N40" s="12">
         <v>3</v>
       </c>
-      <c r="N39" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6539861065167053E-5</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="2"/>
-        <v>3.3112582781456954E-4</v>
-      </c>
-      <c r="D40">
-        <v>30.23</v>
-      </c>
-      <c r="E40">
-        <v>1.51</v>
-      </c>
-      <c r="F40">
-        <v>582</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H40" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I40" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J40">
-        <v>886</v>
-      </c>
-      <c r="K40">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L40">
-        <v>4.4242549593716838E-19</v>
-      </c>
-      <c r="M40">
-        <v>3</v>
-      </c>
-      <c r="N40" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41">
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="11">
         <f>0.0005/D41</f>
         <v>1.7768301350390903E-5</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="11">
         <f>0.0005/E41</f>
         <v>4.8543689320388347E-4</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="12">
         <v>28.14</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="12">
         <v>1.03</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="12">
         <v>582</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="12">
         <v>886</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="11">
+        <f>F41/H41</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L41" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L41">
+      <c r="M41" s="12">
         <v>6.7141516307161576E-19</v>
       </c>
-      <c r="M41">
+      <c r="N41" s="12">
         <v>4</v>
       </c>
-      <c r="N41" s="1">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11">
+        <f t="shared" ref="B42:B48" si="2">0.0005/D42</f>
+        <v>1.4667057788207684E-5</v>
+      </c>
+      <c r="C42" s="11">
+        <f t="shared" ref="C42:C48" si="3">0.0005/E42</f>
+        <v>3.4965034965034965E-4</v>
+      </c>
+      <c r="D42" s="12">
+        <v>34.090000000000003</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1.43</v>
+      </c>
+      <c r="F42" s="12">
+        <v>582</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H42" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I42" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J42" s="12">
+        <v>886</v>
+      </c>
+      <c r="K42" s="11">
+        <f>F42/H42</f>
         <v>76578.947368421053</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" s="1">
-        <f t="shared" ref="B42:B48" si="3">0.0005/D42</f>
-        <v>1.4667057788207684E-5</v>
-      </c>
-      <c r="C42" s="1">
-        <f t="shared" ref="C42:C48" si="4">0.0005/E42</f>
-        <v>3.4965034965034965E-4</v>
-      </c>
-      <c r="D42">
-        <v>34.090000000000003</v>
-      </c>
-      <c r="E42">
-        <v>1.43</v>
-      </c>
-      <c r="F42">
+      <c r="L42" s="12">
+        <v>94472.244000000006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4912019087384431E-5</v>
+      </c>
+      <c r="C43" s="11">
+        <f t="shared" si="3"/>
+        <v>2.0746887966804979E-4</v>
+      </c>
+      <c r="D43" s="12">
+        <v>33.53</v>
+      </c>
+      <c r="E43" s="12">
+        <v>2.41</v>
+      </c>
+      <c r="F43" s="12">
         <v>582</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G43" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H43" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I43" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J42">
+      <c r="J43" s="12">
         <v>886</v>
       </c>
-      <c r="K42">
+      <c r="K43" s="11">
+        <f>F43/H43</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L43" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="N42" s="1">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>43</v>
+      </c>
+      <c r="B44" s="11">
+        <f t="shared" si="2"/>
+        <v>1.6622340425531915E-5</v>
+      </c>
+      <c r="C44" s="11">
+        <f t="shared" si="3"/>
+        <v>2.1008403361344539E-4</v>
+      </c>
+      <c r="D44" s="12">
+        <v>30.08</v>
+      </c>
+      <c r="E44" s="12">
+        <v>2.38</v>
+      </c>
+      <c r="F44" s="12">
+        <v>582</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1.8199999999999999E-5</v>
+      </c>
+      <c r="H44" s="11">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I44" s="11">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J44" s="12">
+        <v>886</v>
+      </c>
+      <c r="K44" s="11">
+        <f>F44/H44</f>
         <v>76578.947368421053</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1">
+      <c r="L44" s="12">
+        <v>94472.244000000006</v>
+      </c>
+      <c r="M44" s="12">
+        <v>2.8945154061813598E-19</v>
+      </c>
+      <c r="N44" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>44</v>
+      </c>
+      <c r="B45" s="11">
+        <f t="shared" si="2"/>
+        <v>1.7674089784376105E-5</v>
+      </c>
+      <c r="C45" s="11">
         <f t="shared" si="3"/>
-        <v>1.4912019087384431E-5</v>
-      </c>
-      <c r="C43" s="1">
-        <f t="shared" si="4"/>
-        <v>2.0746887966804979E-4</v>
-      </c>
-      <c r="D43">
-        <v>33.53</v>
-      </c>
-      <c r="E43">
-        <v>2.41</v>
-      </c>
-      <c r="F43">
+        <v>1.0351966873706004E-4</v>
+      </c>
+      <c r="D45" s="12">
+        <v>28.29</v>
+      </c>
+      <c r="E45" s="12">
+        <v>4.83</v>
+      </c>
+      <c r="F45" s="12">
         <v>582</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G45" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H45" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I45" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J43">
+      <c r="J45" s="12">
         <v>886</v>
       </c>
-      <c r="K43">
+      <c r="K45" s="11">
+        <f>F45/H45</f>
+        <v>76578.947368421053</v>
+      </c>
+      <c r="L45" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="N43" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1">
+      <c r="M45" s="12">
+        <v>1.611410157598895E-19</v>
+      </c>
+      <c r="N45" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>45</v>
+      </c>
+      <c r="B46" s="11">
+        <f t="shared" si="2"/>
+        <v>7.8210542781166897E-6</v>
+      </c>
+      <c r="C46" s="11">
         <f t="shared" si="3"/>
-        <v>1.6622340425531915E-5</v>
-      </c>
-      <c r="C44" s="1">
-        <f t="shared" si="4"/>
-        <v>2.1008403361344539E-4</v>
-      </c>
-      <c r="D44">
-        <v>30.08</v>
-      </c>
-      <c r="E44">
-        <v>2.38</v>
-      </c>
-      <c r="F44">
-        <v>582</v>
-      </c>
-      <c r="G44" s="1">
+        <v>3.0120481927710846E-4</v>
+      </c>
+      <c r="D46" s="12">
+        <v>63.93</v>
+      </c>
+      <c r="E46" s="12">
+        <v>1.66</v>
+      </c>
+      <c r="F46" s="12">
+        <v>583</v>
+      </c>
+      <c r="G46" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H46" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I46" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J44">
+      <c r="J46" s="12">
         <v>886</v>
       </c>
-      <c r="K44">
+      <c r="K46" s="11">
+        <f>F46/H46</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L46" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L44">
-        <v>2.8945154061813598E-19</v>
-      </c>
-      <c r="M44">
-        <v>2</v>
-      </c>
-      <c r="N44" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1">
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="11">
+        <f t="shared" si="2"/>
+        <v>7.9567154678548696E-6</v>
+      </c>
+      <c r="C47" s="11">
         <f t="shared" si="3"/>
-        <v>1.7674089784376105E-5</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" si="4"/>
-        <v>1.0351966873706004E-4</v>
-      </c>
-      <c r="D45">
-        <v>28.29</v>
-      </c>
-      <c r="E45">
-        <v>4.83</v>
-      </c>
-      <c r="F45">
-        <v>582</v>
-      </c>
-      <c r="G45" s="1">
+        <v>2.136752136752137E-4</v>
+      </c>
+      <c r="D47" s="12">
+        <v>62.84</v>
+      </c>
+      <c r="E47" s="12">
+        <v>2.34</v>
+      </c>
+      <c r="F47" s="12">
+        <v>583</v>
+      </c>
+      <c r="G47" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H47" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I47" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J45">
+      <c r="J47" s="12">
         <v>886</v>
       </c>
-      <c r="K45">
+      <c r="K47" s="11">
+        <f>F47/H47</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L47" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="L45">
-        <v>1.611410157598895E-19</v>
-      </c>
-      <c r="M45">
+      <c r="M47" s="12">
+        <v>1.690280283048925E-19</v>
+      </c>
+      <c r="N47" s="12">
         <v>1</v>
       </c>
-      <c r="N45" s="1">
-        <f t="shared" si="0"/>
-        <v>76578.947368421053</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1">
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>47</v>
+      </c>
+      <c r="B48" s="11">
+        <f t="shared" si="2"/>
+        <v>8.0606158310494929E-6</v>
+      </c>
+      <c r="C48" s="11">
         <f t="shared" si="3"/>
-        <v>7.8210542781166897E-6</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" si="4"/>
-        <v>3.0120481927710846E-4</v>
-      </c>
-      <c r="D46">
-        <v>63.93</v>
-      </c>
-      <c r="E46">
-        <v>1.66</v>
-      </c>
-      <c r="F46">
+        <v>6.0240963855421692E-4</v>
+      </c>
+      <c r="D48" s="12">
+        <v>62.03</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0.83</v>
+      </c>
+      <c r="F48" s="12">
         <v>583</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G48" s="11">
         <v>1.8199999999999999E-5</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H48" s="11">
         <v>7.6E-3</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I48" s="11">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="J46">
+      <c r="J48" s="12">
         <v>886</v>
       </c>
-      <c r="K46">
+      <c r="K48" s="11">
+        <f>F48/H48</f>
+        <v>76710.526315789481</v>
+      </c>
+      <c r="L48" s="12">
         <v>94472.244000000006</v>
       </c>
-      <c r="N46" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1">
-        <f t="shared" si="3"/>
-        <v>7.9567154678548696E-6</v>
-      </c>
-      <c r="C47" s="1">
-        <f t="shared" si="4"/>
-        <v>2.136752136752137E-4</v>
-      </c>
-      <c r="D47">
-        <v>62.84</v>
-      </c>
-      <c r="E47">
-        <v>2.34</v>
-      </c>
-      <c r="F47">
-        <v>583</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H47" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I47" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J47">
-        <v>886</v>
-      </c>
-      <c r="K47">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L47">
-        <v>1.690280283048925E-19</v>
-      </c>
-      <c r="M47">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1">
-        <f t="shared" si="3"/>
-        <v>8.0606158310494929E-6</v>
-      </c>
-      <c r="C48" s="1">
-        <f t="shared" si="4"/>
-        <v>6.0240963855421692E-4</v>
-      </c>
-      <c r="D48">
-        <v>62.03</v>
-      </c>
-      <c r="E48">
-        <v>0.83</v>
-      </c>
-      <c r="F48">
-        <v>583</v>
-      </c>
-      <c r="G48" s="1">
-        <v>1.8199999999999999E-5</v>
-      </c>
-      <c r="H48" s="1">
-        <v>7.6E-3</v>
-      </c>
-      <c r="I48" s="1">
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="J48">
-        <v>886</v>
-      </c>
-      <c r="K48">
-        <v>94472.244000000006</v>
-      </c>
-      <c r="L48">
+      <c r="M48" s="12">
         <v>4.7003150270511174E-19</v>
       </c>
-      <c r="M48">
+      <c r="N48" s="12">
         <v>3</v>
       </c>
-      <c r="N48" s="1">
-        <f t="shared" si="0"/>
-        <v>76710.526315789481</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="L49">
-        <f>SUM(L2:L48)</f>
+    </row>
+    <row r="49" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16">
+        <f>SUM(M2:M48)</f>
         <v>9.3129085708425031E-18</v>
       </c>
-      <c r="M49">
-        <f>SUM(M2:M48)</f>
+      <c r="N49" s="16">
+        <f>SUM(N2:N48)</f>
         <v>60</v>
       </c>
-      <c r="N49" t="s">
+      <c r="P49" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O49" t="s">
+      <c r="Q49" s="17">
+        <f>M49/N49</f>
+        <v>1.5521514284737505E-19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="P50" t="s">
         <v>14</v>
       </c>
-      <c r="P49">
-        <f>L49/M49</f>
-        <v>1.5521514284737505E-19</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="O50" t="s">
+      <c r="Q50">
+        <f>1.602176634E-19-Q49</f>
+        <v>5.0025205526249379E-21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="P51" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P50">
-        <f>1.602176634E-19-P49</f>
-        <v>5.0025205526249379E-21</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="O51" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="P51" s="8">
-        <f>P50/P49</f>
+      <c r="Q51" s="5">
+        <f>Q50/Q49</f>
         <v>3.2229590881760667E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="53" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -5403,18 +5520,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>76000</v>
@@ -5422,14 +5539,14 @@
       <c r="C2">
         <v>520</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <f>C2/B2</f>
         <v>6.842105263157895E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>3.7</v>
@@ -5437,14 +5554,14 @@
       <c r="C3">
         <v>0.1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D10" si="0">C3/B3</f>
         <v>2.7027027027027029E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>32.6</v>
@@ -5452,14 +5569,14 @@
       <c r="C4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>3.0674846625766872E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>5.0000000000000001E-4</v>
@@ -5467,30 +5584,30 @@
       <c r="C5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
         <v>4.7E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3">
         <v>2.3099999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>94000</v>
@@ -5498,14 +5615,14 @@
       <c r="C8">
         <v>1000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>1.0638297872340425E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <f>SUM(Tabelle1!G2:G48)/COUNT(Tabelle1!G2:G48)</f>
@@ -5514,14 +5631,14 @@
       <c r="C9" s="1">
         <v>1E-8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>5.499262864764933E-4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>886</v>
@@ -5529,14 +5646,14 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>1.128668171557562E-3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>9.81</v>
@@ -5544,14 +5661,14 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f>C11/B11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>8.2000000000000007E-3</v>
@@ -5559,16 +5676,16 @@
       <c r="C12">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <f>C12/B12</f>
         <v>1.2195121951219512E-3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="4">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3">
         <v>0.18429999999999999</v>
       </c>
     </row>

</xml_diff>